<commit_message>
Add bulk paste input for assessment data
Introduces a textarea for users to paste semicolon/comma-separated data from the spreadsheet, with parsing and validation logic. Table population and results generation now use the pasted data, and an example data section is provided for guidance. Removes the reset modal and related callbacks, streamlining the workflow for rapid prototyping.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat DDO Roadmap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1331" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{544E320E-8B6F-4139-8176-5BA223BAA1EB}"/>
+  <xr:revisionPtr revIDLastSave="1528" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A2F92A-451F-43E5-A34F-7ABA31622AA4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagnostic Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -325,12 +325,6 @@
     <t>(1) Yes/No:</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <r>
       <t>Since the adoption of the National Development Strategy, have at least 50% of essential government entities*</t>
     </r>
@@ -396,14 +390,38 @@
     <t>Financial Protection</t>
   </si>
   <si>
-    <t>Number of questions unanswered</t>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cat-ddo-drm-diagnostic-dashboard.onrender.com </t>
+  </si>
+  <si>
+    <t>DRM System - Diagnostic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of questions unanswered: </t>
+  </si>
+  <si>
+    <t>1. Answer the questions in the following matrix.</t>
+  </si>
+  <si>
+    <t>Pillar</t>
+  </si>
+  <si>
+    <t>Subpillar</t>
+  </si>
+  <si>
+    <t>2. Go to the following website. The website may take some time to load. Please retry if needed.</t>
+  </si>
+  <si>
+    <t>3. Copy and Paste Cell E7 to the website</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,19 +552,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -565,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -944,20 +1019,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,418 +1056,423 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1428,7 +1518,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Summary!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1449,7 +1539,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$3:$C$14</c:f>
+              <c:f>Summary!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1494,16 +1584,34 @@
                   <c:pt idx="0">
                     <c:v>Legal and Institutional DRM Framework</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Legal and Institutional DRM Framework</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>Risk Identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Risk Reduction</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
                   <c:pt idx="6">
                     <c:v>Preparedness</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
                   <c:pt idx="9">
+                    <c:v>Financial Protection</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Financial Protection</c:v>
                   </c:pt>
                   <c:pt idx="11">
@@ -1515,33 +1623,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$14</c:f>
+              <c:f>Summary!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1550,10 +1658,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,7 +1677,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Summary!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1590,7 +1698,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$3:$C$14</c:f>
+              <c:f>Summary!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1635,16 +1743,34 @@
                   <c:pt idx="0">
                     <c:v>Legal and Institutional DRM Framework</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Legal and Institutional DRM Framework</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>Risk Identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Risk Reduction</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
                   <c:pt idx="6">
                     <c:v>Preparedness</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
                   <c:pt idx="9">
+                    <c:v>Financial Protection</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Financial Protection</c:v>
                   </c:pt>
                   <c:pt idx="11">
@@ -1656,39 +1782,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$14</c:f>
+              <c:f>Summary!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1710,7 +1836,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Summary!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1731,7 +1857,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$3:$C$14</c:f>
+              <c:f>Summary!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1776,16 +1902,34 @@
                   <c:pt idx="0">
                     <c:v>Legal and Institutional DRM Framework</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Legal and Institutional DRM Framework</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>Risk Identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Risk Reduction</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
                   <c:pt idx="6">
                     <c:v>Preparedness</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
                   <c:pt idx="9">
+                    <c:v>Financial Protection</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Financial Protection</c:v>
                   </c:pt>
                   <c:pt idx="11">
@@ -1797,45 +1941,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$14</c:f>
+              <c:f>Summary!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1851,7 +1995,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Summary!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1872,7 +2016,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$3:$C$14</c:f>
+              <c:f>Summary!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1917,16 +2061,34 @@
                   <c:pt idx="0">
                     <c:v>Legal and Institutional DRM Framework</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Legal and Institutional DRM Framework</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>Risk Identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Risk Reduction</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Risk Reduction</c:v>
+                  </c:pt>
                   <c:pt idx="6">
                     <c:v>Preparedness</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Preparedness</c:v>
+                  </c:pt>
                   <c:pt idx="9">
+                    <c:v>Financial Protection</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Financial Protection</c:v>
                   </c:pt>
                   <c:pt idx="11">
@@ -1938,21 +2100,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$14</c:f>
+              <c:f>Summary!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1961,19 +2123,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -2742,15 +2904,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:colOff>550961</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>70237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>678180</xdr:colOff>
+      <xdr:colOff>611921</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:rowOff>66428</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3099,1126 +3261,1005 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E233A1B-F2D0-419A-984D-979291E6494E}">
-  <dimension ref="A5:AU49"/>
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="B2:AU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:R25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="41.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="24" customWidth="1"/>
     <col min="6" max="6" width="54.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="24" customWidth="1"/>
     <col min="8" max="8" width="65" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" style="37" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="24" customWidth="1"/>
     <col min="10" max="10" width="55.5546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" style="37" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" style="24" customWidth="1"/>
     <col min="12" max="12" width="38.88671875" customWidth="1"/>
     <col min="13" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="47" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:47" s="2" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7"/>
-      <c r="B7" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="65" t="s">
+    <row r="2" spans="2:47" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="141" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:47" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:47" x14ac:dyDescent="0.35">
+      <c r="B4" s="143" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:47" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="144" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="145" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="145"/>
+    </row>
+    <row r="7" spans="2:47" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="146" t="str">
+        <f>_xlfn.TEXTJOIN(";",FALSE,Summary!I2:I14)</f>
+        <v>Pillar,Subpillar,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0;Risk Identification,Risk Identification,0,0,0,0;Risk Reduction,Territorial and urban planning,0,0,0,0;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0,0,0,0;Preparedness,Early Warning Systems (EWS),0,0,0,0;Preparedness,Emergency Preparedness and Response (EP&amp;R),0,0,0,0;Preparedness,Adaptive Social Protection (ASP),0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,Disaster Risk Financing (DRF) strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient Reconstruction,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:47" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="67">
+        <f>64-(COUNTIF('Diagnostic Questions'!D12:K50,"YES")+COUNTIF('Diagnostic Questions'!D12:K50,"NO"))</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:47" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="142" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:47" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:47" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D12" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="66" t="s">
+      <c r="E12" s="131"/>
+      <c r="F12" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="66" t="s">
+      <c r="G12" s="131"/>
+      <c r="H12" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="66" t="s">
+      <c r="I12" s="131"/>
+      <c r="J12" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-    </row>
-    <row r="8" spans="1:47" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="39" t="s">
+      <c r="K12" s="130"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+    </row>
+    <row r="13" spans="2:47" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="94" t="s">
+      <c r="D13" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="105"/>
-      <c r="F8" s="94" t="s">
+      <c r="E13" s="132"/>
+      <c r="F13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="105"/>
-      <c r="H8" s="106" t="s">
+      <c r="G13" s="132"/>
+      <c r="H13" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="107"/>
-      <c r="J8" s="106" t="s">
+      <c r="I13" s="133"/>
+      <c r="J13" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="108"/>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" spans="1:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="111" t="s">
+      <c r="K13" s="128"/>
+      <c r="L13" s="25"/>
+    </row>
+    <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="69"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="143" t="s">
+      <c r="E14" s="66"/>
+      <c r="F14" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="69"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="69"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="50"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="69"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="69"/>
+      <c r="C18" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="117"/>
+      <c r="F18" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="117"/>
+      <c r="H18" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="I18" s="120"/>
+      <c r="J18" s="116" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="121"/>
+      <c r="L18" s="34"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="70"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="43" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="20"/>
+      <c r="L19" s="35"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="111" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="115"/>
+      <c r="F20" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="115"/>
+      <c r="H20" s="114" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="115"/>
+      <c r="J20" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="124"/>
+      <c r="L20" s="25"/>
+    </row>
+    <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="112"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J9" s="43" t="s">
+      <c r="G21" s="11"/>
+      <c r="H21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="25"/>
+    </row>
+    <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="113"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="25"/>
+    </row>
+    <row r="23" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="122" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="87"/>
+      <c r="F23" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="87"/>
+      <c r="H23" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="87"/>
+      <c r="J23" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="126"/>
+      <c r="L23" s="25"/>
+    </row>
+    <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="69"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="69"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="25"/>
+    </row>
+    <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="69"/>
+      <c r="C26" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="84"/>
+      <c r="F26" s="83" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="84"/>
+      <c r="H26" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="84"/>
+      <c r="J26" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="77"/>
+      <c r="L26" s="25"/>
+    </row>
+    <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="69"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" s="38"/>
-    </row>
-    <row r="10" spans="1:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="116"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="43" t="s">
+      <c r="K27" s="18"/>
+      <c r="L27" s="25"/>
+    </row>
+    <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="69"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L10" s="38"/>
-    </row>
-    <row r="11" spans="1:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="50" t="s">
+      <c r="K28" s="23"/>
+      <c r="L28" s="25"/>
+    </row>
+    <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="69"/>
+      <c r="C29" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="76"/>
+      <c r="F29" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="85"/>
+      <c r="H29" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="76"/>
+      <c r="J29" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="77"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="69"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="69"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" s="121" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="38"/>
-    </row>
-    <row r="12" spans="1:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="38"/>
-    </row>
-    <row r="13" spans="1:47" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="100"/>
-      <c r="H13" s="101" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="103" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="104"/>
-      <c r="L13" s="61"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:47" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="69"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="69"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="69"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="97"/>
+      <c r="F34" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="76"/>
+      <c r="H34" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="85"/>
+      <c r="J34" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="98"/>
+      <c r="L34" s="25"/>
+    </row>
+    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="69"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="47" t="s">
+      <c r="E35" s="11"/>
+      <c r="F35" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="47" t="s">
+      <c r="G35" s="11"/>
+      <c r="H35" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="47" t="s">
+      <c r="K35" s="18"/>
+      <c r="L35" s="25"/>
+    </row>
+    <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="70"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="19"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="25"/>
+    </row>
+    <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="111" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="108" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="79"/>
+      <c r="F37" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="79"/>
+      <c r="H37" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="79"/>
+      <c r="J37" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" s="99"/>
+      <c r="L37" s="36"/>
+    </row>
+    <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="112"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="L14" s="62"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:47" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="E38" s="22"/>
+      <c r="F38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="22"/>
+      <c r="H38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="20"/>
+      <c r="L38" s="36"/>
+    </row>
+    <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="112"/>
+      <c r="C39" s="135" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="101"/>
+      <c r="F39" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="101"/>
+      <c r="H39" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="107"/>
+      <c r="J39" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" s="103"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="112"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="18"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="112"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="22"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="64"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="112"/>
+      <c r="C42" s="135" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="101"/>
+      <c r="F42" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="101"/>
+      <c r="H42" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="105"/>
+      <c r="J42" s="100" t="s">
+        <v>52</v>
+      </c>
+      <c r="K42" s="104"/>
+      <c r="L42" s="25"/>
+    </row>
+    <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="113"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="19"/>
+      <c r="H43" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" s="19"/>
+      <c r="J43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="20"/>
+      <c r="L43" s="25"/>
+    </row>
+    <row r="44" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="122" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="87"/>
+      <c r="F44" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="87"/>
+      <c r="H44" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="I44" s="87"/>
+      <c r="J44" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="K44" s="93"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="69"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="22"/>
+      <c r="H45" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="22"/>
+      <c r="J45" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="23"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="69"/>
+      <c r="C46" s="138" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="88"/>
+      <c r="F46" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="G46" s="92"/>
+      <c r="H46" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="88"/>
+      <c r="J46" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="94"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="69"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="18"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="70"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="19"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="111" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="97"/>
-      <c r="F15" s="96" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="96" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="97"/>
-      <c r="J15" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="98"/>
-      <c r="L15" s="38"/>
-    </row>
-    <row r="16" spans="1:47" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="14" t="s">
+      <c r="D49" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="79"/>
+      <c r="F49" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="90"/>
+      <c r="H49" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="I49" s="79"/>
+      <c r="J49" s="95" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" s="96"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="113"/>
+      <c r="C50" s="137"/>
+      <c r="D50" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="E50" s="19"/>
+      <c r="F50" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="14" t="s">
+      <c r="G50" s="19"/>
+      <c r="H50" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="L16" s="38"/>
-    </row>
-    <row r="17" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="130"/>
-      <c r="F17" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="124"/>
-      <c r="I17" s="130"/>
-      <c r="J17" s="124"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="38"/>
-    </row>
-    <row r="18" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="70"/>
-      <c r="F18" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="70"/>
-      <c r="H18" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="95"/>
-      <c r="L18" s="38"/>
-    </row>
-    <row r="19" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="43" t="s">
+      <c r="I50" s="19"/>
+      <c r="J50" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J19" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L19" s="38"/>
-    </row>
-    <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="41"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="115"/>
-      <c r="I20" s="119"/>
-      <c r="J20" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="2:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
-      <c r="C21" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="93"/>
-      <c r="F21" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="93"/>
-      <c r="H21" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="93"/>
-      <c r="J21" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="92"/>
-      <c r="L21" s="38"/>
-    </row>
-    <row r="22" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="K22" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L22" s="38"/>
-    </row>
-    <row r="23" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="41"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="115"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="115"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="K23" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L23" s="38"/>
-    </row>
-    <row r="24" spans="2:13" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="41"/>
-      <c r="C24" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="87" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="89"/>
-      <c r="F24" s="90" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="90"/>
-      <c r="H24" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="89"/>
-      <c r="J24" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" s="92"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="41"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="119" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H25" s="111" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J25" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L25" s="38"/>
-      <c r="M25" s="5"/>
-    </row>
-    <row r="26" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="125"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="119"/>
-      <c r="J26" s="114"/>
-      <c r="K26" s="139"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="41"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="125"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="119"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="139"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="5"/>
-    </row>
-    <row r="28" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="41"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="125"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="113"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="139"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="41"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="88"/>
-      <c r="F29" s="87" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="89"/>
-      <c r="H29" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="90"/>
-      <c r="J29" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="91"/>
-      <c r="L29" s="38"/>
-    </row>
-    <row r="30" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="41"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H30" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J30" s="127" t="s">
-        <v>11</v>
-      </c>
-      <c r="K30" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30" s="38"/>
-    </row>
-    <row r="31" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="142"/>
-      <c r="H31" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J31" s="126"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="38"/>
-    </row>
-    <row r="32" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="85"/>
-      <c r="F32" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="G32" s="85"/>
-      <c r="H32" s="84" t="s">
-        <v>42</v>
-      </c>
-      <c r="I32" s="85"/>
-      <c r="J32" s="84" t="s">
-        <v>43</v>
-      </c>
-      <c r="K32" s="86"/>
-      <c r="L32" s="63"/>
-    </row>
-    <row r="33" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="26"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="L33" s="63"/>
-    </row>
-    <row r="34" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26"/>
-      <c r="C34" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="80" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="78"/>
-      <c r="F34" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="78"/>
-      <c r="H34" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="I34" s="83"/>
-      <c r="J34" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="K34" s="82"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="5"/>
-    </row>
-    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="26"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="L35" s="59"/>
-      <c r="M35" s="5"/>
-    </row>
-    <row r="36" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="26"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="129"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="129"/>
-      <c r="H36" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J36" s="33"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="5"/>
-    </row>
-    <row r="37" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="26"/>
-      <c r="C37" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="78"/>
-      <c r="F37" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="78"/>
-      <c r="H37" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="I37" s="81"/>
-      <c r="J37" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="K37" s="140"/>
-      <c r="L37" s="38"/>
-    </row>
-    <row r="38" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="23"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="K38" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="L38" s="38"/>
-    </row>
-    <row r="39" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="69" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="70"/>
-      <c r="F39" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" s="70"/>
-      <c r="H39" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="I39" s="70"/>
-      <c r="J39" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="K39" s="71"/>
-      <c r="L39" s="59"/>
-    </row>
-    <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="41"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H40" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J40" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="L40" s="59"/>
-    </row>
-    <row r="41" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="41"/>
-      <c r="C41" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="73"/>
-      <c r="F41" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="G41" s="75"/>
-      <c r="H41" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="73"/>
-      <c r="J41" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="K41" s="76"/>
-      <c r="L41" s="59"/>
-    </row>
-    <row r="42" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="41"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42" s="127" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K42" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="L42" s="59"/>
-    </row>
-    <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="45"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="126"/>
-      <c r="E43" s="137"/>
-      <c r="F43" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H43" s="128"/>
-      <c r="I43" s="137"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="138"/>
-      <c r="L43" s="59"/>
-    </row>
-    <row r="44" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="85"/>
-      <c r="F44" s="132" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44" s="133"/>
-      <c r="H44" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="I44" s="85"/>
-      <c r="J44" s="134" t="s">
-        <v>68</v>
-      </c>
-      <c r="K44" s="135"/>
-      <c r="L44" s="59"/>
-    </row>
-    <row r="45" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="J45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K45" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="L45" s="59"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D46" s="13"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="36"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D47" s="13"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="36"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D48" s="13"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="36"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D49" s="13"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="36"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B18:B31"/>
-    <mergeCell ref="C24:C31"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H21:I21"/>
+  <mergeCells count="76">
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H34:I34"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B23:B36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="B8:B14"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K22:K23 G9 E9 E14 G14 I14 K14 I11 G16:G17 K9:K11 E16 I16 K16 I19 G19 E19 E22 G22 G25 E30 I30:I31 G35 E35 K30 K35 E42 I42 E25:E28 G30 I33 K33 G33 E33 I35:I36 K38 I38 G38 E38 E40 E45 G45 G42:G43 I45 K45 K40 I40 G40 I25 K25 I22 K19:K20 I9 K42" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K27:K28 G14 E14 E19 G19 I19 K19 I16 G21:G22 K14:K16 E21 I21 K21 I24 G24 E24 E27 G27 G30 E35 I35:I36 G40 E40 K35 K40 E47 I47 E30:E33 G35 I38 K38 G38 E38 I40:I41 K43 I43 G43 E43 E45 E50 G50 G47:G48 I50 K50 K45 I45 G45 I30 K30 I27 K24:K25 I14 K47" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{1CA86482-C762-4B74-AE4C-5776DD22645C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;R_x000D_&amp;1#&amp;"Aptos"&amp;10&amp;K000000 Official Use Only</oddFooter>
   </headerFooter>
@@ -4227,10 +4268,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F2FEA7-2755-42AA-AE92-AD811EBA4B74}">
-  <dimension ref="B2:G16"/>
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4238,312 +4282,373 @@
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="110" t="s">
+    <row r="2" spans="2:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="110" t="s">
+      <c r="F2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="109" t="s">
+      <c r="I2" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,B2:G2)</f>
+        <v>Pillar,Subpillar,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="39">
+        <f>IF('Diagnostic Questions'!E14="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>IF('Diagnostic Questions'!G14="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="39">
+        <f>0.5*IF('Diagnostic Questions'!I14="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I16="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="39">
+        <f>ROUND(0.3333*IF('Diagnostic Questions'!K14="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K15="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K16="Yes",1,0),2)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,B3:G3)</f>
+        <v>Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="39">
+        <f>IF('Diagnostic Questions'!E19="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="39">
+        <f>IF('Diagnostic Questions'!G19="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="39">
+        <f>IF('Diagnostic Questions'!I19="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="39">
+        <f>IF('Diagnostic Questions'!K19="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,B4:G4)</f>
+        <v>Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="39">
+        <f>IF('Diagnostic Questions'!E21="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="39">
+        <f>0.5*IF('Diagnostic Questions'!G21="Yes",1,0) + 0.5*IF('Diagnostic Questions'!G22="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="39">
+        <f>IF('Diagnostic Questions'!I21="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="39">
+        <f>IF('Diagnostic Questions'!K21="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:I14" si="0">_xlfn.TEXTJOIN(",",FALSE,B5:G5)</f>
+        <v>Risk Identification,Risk Identification,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="39">
+        <f>IF('Diagnostic Questions'!E24="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="39">
+        <f>IF('Diagnostic Questions'!G24="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="39">
+        <f>IF('Diagnostic Questions'!I24="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="39">
+        <f>0.5*IF('Diagnostic Questions'!K24="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K25="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>Risk Reduction,Territorial and urban planning,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="39">
+        <f>IF('Diagnostic Questions'!E27="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="39">
+        <f>IF('Diagnostic Questions'!G27="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="39">
+        <f>IF('Diagnostic Questions'!I27="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="39">
+        <f>0.5*IF('Diagnostic Questions'!K27="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K28="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Risk Reduction,Public investment at the central level,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="39">
+        <f>0.5*(0.25*IF('Diagnostic Questions'!E30="Yes",1,0)+0.25*IF('Diagnostic Questions'!E31="Yes",1,0)+0.25*IF('Diagnostic Questions'!E32="Yes",1,0)+0.25*IF('Diagnostic Questions'!E33="Yes",1,0))+0.5*IF('Diagnostic Questions'!E35="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="39">
+        <f>0.5*IF('Diagnostic Questions'!G30="Yes",1,0)+0.5*IF('Diagnostic Questions'!G35="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="39">
+        <f>0.5*IF('Diagnostic Questions'!I30="Yes",1,0)+0.5*(0.5*IF('Diagnostic Questions'!I35="Yes",1,0)+0.5*IF('Diagnostic Questions'!I36="Yes",1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="39">
+        <f>0.5*IF('Diagnostic Questions'!K30="Yes",1,0)+0.5*IF('Diagnostic Questions'!K35="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Risk Reduction,Sector-specific risk reduction measures,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="109" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="109">
-        <f>IF(Questions!E9="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f>IF(Questions!G9="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="109">
-        <f>0.5*IF(Questions!I9="Yes",1,0) + 0.5*IF(Questions!I11="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="109">
-        <f>ROUND(0.3333*IF(Questions!K9="Yes",1,0) + 0.3333*IF(Questions!K10="Yes",1,0) + 0.3333*IF(Questions!K11="Yes",1,0),2)</f>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="109"/>
-      <c r="C4" s="109" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="109">
-        <f>IF(Questions!E14="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="109">
-        <f>IF(Questions!G14="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="109">
-        <f>IF(Questions!I14="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="109">
-        <f>IF(Questions!K14="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="109" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="109" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="109">
-        <f>IF(Questions!E16="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="109">
-        <f>0.5*IF(Questions!G16="Yes",1,0) + 0.5*IF(Questions!G17="Yes",1,0)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="109">
-        <f>IF(Questions!I16="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="109">
-        <f>IF(Questions!K16="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="109" t="s">
+      <c r="C9" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="39">
+        <f>IF('Diagnostic Questions'!E38="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="39">
+        <f>IF('Diagnostic Questions'!G38="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="39">
+        <f>IF('Diagnostic Questions'!I38="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="39">
+        <f>IF('Diagnostic Questions'!K38="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>Preparedness,Early Warning Systems (EWS),0,0,0,0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="39">
+        <f>IF('Diagnostic Questions'!E40="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="39">
+        <f>IF('Diagnostic Questions'!G40="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="39">
+        <f>0.5*IF('Diagnostic Questions'!I40="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I41="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="39">
+        <f>IF('Diagnostic Questions'!K40="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>Preparedness,Emergency Preparedness and Response (EP&amp;R),0,0,0,0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="39">
+        <f>IF('Diagnostic Questions'!E43="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="39">
+        <f>IF('Diagnostic Questions'!G43="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="39">
+        <f>IF('Diagnostic Questions'!I43="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="39">
+        <f>IF('Diagnostic Questions'!K43="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>Preparedness,Adaptive Social Protection (ASP),0,0,0,0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="109" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="109">
-        <f>IF(Questions!E19="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="109">
-        <f>IF(Questions!G19="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="109">
-        <f>IF(Questions!I19="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="109">
-        <f>0.5*IF(Questions!K19="Yes",1,0) + 0.5*IF(Questions!K20="Yes",1,0)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="109"/>
-      <c r="C7" s="109" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="109">
-        <f>IF(Questions!E22="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="109">
-        <f>IF(Questions!G22="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="109">
-        <f>IF(Questions!I22="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="109">
-        <f>0.5*IF(Questions!K22="Yes",1,0) + 0.5*IF(Questions!K23="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="109"/>
-      <c r="C8" s="109" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="109">
-        <f>0.5*(0.25*IF(Questions!E25="Yes",1,0)+0.25*IF(Questions!E26="Yes",1,0)+0.25*IF(Questions!E27="Yes",1,0)+0.25*IF(Questions!E28="Yes",1,0))+0.5*IF(Questions!E30="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="109">
-        <f>0.5*IF(Questions!G25="Yes",1,0)+0.5*IF(Questions!G30="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="109">
-        <f>0.5*IF(Questions!I25="Yes",1,0)+0.5*(0.5*IF(Questions!I30="Yes",1,0)+0.5*IF(Questions!I31="Yes",1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="109">
-        <f>0.5*IF(Questions!K25="Yes",1,0)+0.5*IF(Questions!K30="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="109" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="109" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="109">
-        <f>IF(Questions!E33="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="109">
-        <f>IF(Questions!G33="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="109">
-        <f>IF(Questions!I33="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="109">
-        <f>IF(Questions!K33="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="109"/>
-      <c r="C10" s="109" t="s">
+      <c r="C12" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="109">
-        <f>IF(Questions!E35="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="109">
-        <f>IF(Questions!G35="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="109">
-        <f>0.5*IF(Questions!I35="Yes",1,0) + 0.5*IF(Questions!I36="Yes",1,0)</f>
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="109">
-        <f>IF(Questions!K35="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="109"/>
-      <c r="C11" s="109" t="s">
+      <c r="D12" s="39">
+        <f>IF('Diagnostic Questions'!E45="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="39">
+        <f>IF('Diagnostic Questions'!G45="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="39">
+        <f>IF('Diagnostic Questions'!I45="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="39">
+        <f>IF('Diagnostic Questions'!K45="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>Financial Protection,Fiscal risk management,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="109">
-        <f>IF(Questions!E38="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="109">
-        <f>IF(Questions!G38="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="109">
-        <f>IF(Questions!I38="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="109">
-        <f>IF(Questions!K38="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="109" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="109" t="s">
+      <c r="D13" s="39">
+        <f>IF('Diagnostic Questions'!E47="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="39">
+        <f>0.5*IF('Diagnostic Questions'!G47="Yes",1,0)+0.5*IF('Diagnostic Questions'!G48="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="39">
+        <f>IF('Diagnostic Questions'!I47="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="39">
+        <f>IF('Diagnostic Questions'!K47="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>Financial Protection,Disaster Risk Financing (DRF) strategies and instruments,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="109">
-        <f>IF(Questions!E40="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="109">
-        <f>IF(Questions!G40="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="109">
-        <f>IF(Questions!I40="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="109">
-        <f>IF(Questions!K40="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="109"/>
-      <c r="C13" s="109" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="109">
-        <f>IF(Questions!E42="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="109">
-        <f>0.5*IF(Questions!G42="Yes",1,0)+0.5*IF(Questions!G43="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="109">
-        <f>IF(Questions!I42="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="109">
-        <f>IF(Questions!K42="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="109" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="109" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="109">
-        <f>IF(Questions!E45="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="109">
-        <f>IF(Questions!G45="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="109">
-        <f>IF(Questions!I45="Yes",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="109">
-        <f>IF(Questions!K45="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="144">
-        <f>64-(COUNTIF(Questions!D7:K45,"YES")+COUNTIF(Questions!D7:K45,"NO"))</f>
-        <v>0</v>
-      </c>
+      <c r="C14" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="39">
+        <f>IF('Diagnostic Questions'!E50="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="39">
+        <f>IF('Diagnostic Questions'!G50="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="39">
+        <f>IF('Diagnostic Questions'!I50="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="39">
+        <f>IF('Diagnostic Questions'!K50="Yes",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>Resilient Reconstruction,Resilient Reconstruction,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor sub-pillar to Thematic Area in assessment app
Replaces 'DRM sub-pillar' with 'Thematic Area' across app.py, data templates, and figure generation logic for consistency. Updates example data, parsing, and UI labels to match new terminology and structure. Cleans up unused code and improves clarity in table and results presentation.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1528" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A2F92A-451F-43E5-A34F-7ABA31622AA4}"/>
+  <xr:revisionPtr revIDLastSave="1609" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDDBB970-0B64-4DE6-B91C-21E2C866740E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagnostic Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Summary (to be hidden)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="110">
   <si>
     <t>DRM Pillar</t>
   </si>
   <si>
-    <t>DRM sub-pillar</t>
-  </si>
-  <si>
     <t>Legal and institutional set up</t>
   </si>
   <si>
@@ -60,22 +57,9 @@
     <t>1.1. DRM policies and institutions</t>
   </si>
   <si>
-    <t>Is there a legal framework (e.g., DRM law or others) defining distinct mandates for, on the one hand, disaster risk reduction and, on the other, emergency management?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Did the institution responsible for coordinating or leading DRM activities receive dedicated funding for these functions in the last fiscal year? </t>
   </si>
   <si>
-    <t xml:space="preserve">Since the adoption of the DRM legal framework: 
-(1) have DRM policy instruments (e.g., DRM strategies or policies) been officially approved? 
-(2)  have DRM-related regulations (e.g., rules on the structure or functions of the DRM agency) been officially approved? If yes, please specify which policy document(s) and/or regulation(s). </t>
-  </si>
-  <si>
-    <t>(1) Are gender-specific considerations included in DRM legal frameworks? 
-(2) Is climate change and its potential impact on disaster risk included in DRM legal frameworks? 
-(3) When they exist, do climate change laws and regulations (such as climate laws or climate adaptation policy/strategies) contain disaster risk management as a target, aim, mean or result?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes/No: </t>
   </si>
   <si>
@@ -83,9 +67,6 @@
   </si>
   <si>
     <t>Does the National Development Strategy (or equivalent national planning instrument) contain objectives, targets or indicators related to DRM and/or CCA?</t>
-  </si>
-  <si>
-    <t>Is there a reporting or monitoring mechanism to track progress toward DRM and/or CCA targets included in the National Development Strategies? If yes, please report those progress</t>
   </si>
   <si>
     <t xml:space="preserve">Is the integration of DRM considerations into sectoral planning documents coordinated at the central level and guided by norms and clear standards? </t>
@@ -111,9 +92,6 @@
     <t>3.1. Territorial and urban planning</t>
   </si>
   <si>
-    <t>Do laws and regulations mandate the use of risk information (e.g., hazard maps, risk assessments...) to develop territorial, spatial, land use or urban planning instruments?</t>
-  </si>
-  <si>
     <t>Do official methodologies to guide the development of risk-informed territorial, spatial, land use or urban planning instruments exist?</t>
   </si>
   <si>
@@ -128,9 +106,6 @@
   </si>
   <si>
     <t>Do laws and regulations mandate disaster and climate risk screening as part of the appraisal of new public investment projects?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do official guidelines defining disaster and climate risk screening methodologies for new public investment projects exist? </t>
   </si>
   <si>
     <t>Are risk mitigation measures in place for new projects that have been appraised as high-risk (or equivalent) through the disaster and climate screening process?</t>
@@ -156,12 +131,6 @@
     <t>Is there an asset management system for public infrastructure that includes disaster risk analysis?</t>
   </si>
   <si>
-    <t xml:space="preserve">Is the legal framework and institutional arrangements for water supply and sanitation in urban areas considering flood risk? </t>
-  </si>
-  <si>
-    <t>Is there a legal framework and institutional arrangements for integrated water resources management (IWRM) that explicitly incorporates flood and drought risk considerations?</t>
-  </si>
-  <si>
     <t>Over the last 4 years: 
 (1) have any watershed basins undergone improvements in water management?
 (2) has the percentage of urban residents with access to sewage services been maintained or increased?</t>
@@ -206,9 +175,6 @@
     <t>Is there a unified social registry incorporating exposure and vulnerability data to facilitate the targeting of population potentially affected in case of disaster or climate-related shocks?</t>
   </si>
   <si>
-    <t>During the most recent disaster or climate-related shocks, was support promptly provided to the population through social‐protection programs?  (e.g., cash transfers in the case of drought)?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Are there pre-arranged financing mechanisms that can be specifically used to support timely scaling-up of regular SP programs? </t>
   </si>
   <si>
@@ -224,23 +190,14 @@
     <t>Are contingent liabilities associated with disasters quantified through an established methodology for the major hazards?</t>
   </si>
   <si>
-    <t>Do key fiscal policy documents (e.g., the medium-term fiscal framework or fiscal risk statements) include quantified assessments of disaster risks? If yes, please specify which document(s).</t>
-  </si>
-  <si>
     <t>Has the government conducted stress tests of public debt that include disaster or climate-related scenarios?</t>
   </si>
   <si>
     <t>5.2. Disaster Risk Financing (DRF) strategies and instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are there sovereign risk financing instruments (e.g., disaster or emergency funds, contingent loans, insurance or other risk transfer mechanisms) in place to manage the financial impact of disasters and climate-related shocks? If yes, please list them. </t>
   </si>
   <si>
     <t>(1) Is the disaster fund (or equivalent mechanism) receiving a budget allocation? 
 (2) Are there regulations that define standards for catastrophe insurance coverage of public or private assets?</t>
-  </si>
-  <si>
-    <t>Over the past 4 years, has the $ amount of financing that can be mobilized through sovereign risk financing instruments increased? Please provide numbers when available</t>
   </si>
   <si>
     <t>Is there a legal or policy framework that outlines a layered Disaster Risk Financing (DRF) strategy combining risk retention and risk transfer instruments?</t>
@@ -300,10 +257,6 @@
     <t>Is there a legal framework clearly defining the roles and responsibility of institutions involved in Early Warning Systems, avoiding fragmentation?</t>
   </si>
   <si>
-    <t>(1) Does at least 75% of essential government entities have an emergency response protocol / operational continuity plan? 
-(2) Does at least 75% of subnational EP&amp;R entities have an approved contingency plan / emergency response protocol?</t>
-  </si>
-  <si>
     <t>Intermediary DRM outputs</t>
   </si>
   <si>
@@ -360,21 +313,9 @@
     <t>Sector-specific risk reduction measures</t>
   </si>
   <si>
-    <t>Early Warning Systems (EWS)</t>
-  </si>
-  <si>
-    <t>Emergency Preparedness and Response (EP&amp;R)</t>
-  </si>
-  <si>
-    <t>Adaptive Social Protection (ASP)</t>
-  </si>
-  <si>
     <t>Fiscal risk management</t>
   </si>
   <si>
-    <t>Disaster Risk Financing (DRF) strategies and instruments</t>
-  </si>
-  <si>
     <t>Resilient Reconstruction</t>
   </si>
   <si>
@@ -405,23 +346,143 @@
     <t>1. Answer the questions in the following matrix.</t>
   </si>
   <si>
-    <t>Pillar</t>
-  </si>
-  <si>
-    <t>Subpillar</t>
-  </si>
-  <si>
     <t>2. Go to the following website. The website may take some time to load. Please retry if needed.</t>
   </si>
   <si>
     <t>3. Copy and Paste Cell E7 to the website</t>
+  </si>
+  <si>
+    <t>Thematic Area</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>DRF strategies and instruments</t>
+  </si>
+  <si>
+    <t>Risk identification</t>
+  </si>
+  <si>
+    <t>Early warning systems</t>
+  </si>
+  <si>
+    <t>Emergency preparedness and response</t>
+  </si>
+  <si>
+    <t>Adaptive social protection</t>
+  </si>
+  <si>
+    <t>Resilient reconstruction</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Is there a legal framework (e.g., a DRM law or other instruments) defining distinct mandates for disaster risk reduction and emergency management?</t>
+  </si>
+  <si>
+    <t>(1) Are gender-specific considerations included in DRM legal frameworks? 
+(2) Is climate change and its potential impact on disaster risk included in DRM legal frameworks? 
+(3) When they exist, do climate change laws and regulations (such as climate laws or climate adaptation policy/strategies) contain disaster risk management as a target, aim, means, or result?</t>
+  </si>
+  <si>
+    <t>Do laws and regulations mandate the use of risk information (e.g., hazard maps, risk assessments...) to develop territorial, spatial, land use, or urban planning instruments?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do official guidelines exist defining disaster and climate risk screening methodologies for new public investment projects? </t>
+  </si>
+  <si>
+    <t>Do the legal framework and institutional arrangements for water supply and sanitation in urban areas take flood risk into account?</t>
+  </si>
+  <si>
+    <t>Are there legal and institutional arrangements for integrated water resources management (IWRM) that explicitly incorporate flood and drought risk considerations?</t>
+  </si>
+  <si>
+    <t>(1) Do at least 75% of essential government entities have an emergency response protocol or operational continuity plan? 
+(2) Do at least 75% of subnational EP&amp;R entities have an approved contingency plan or emergency response protocol?</t>
+  </si>
+  <si>
+    <t>During the most recent disaster or climate-related shock, was support promptly provided to the population through social‐protection programs?  (e.g., cash transfers in the case of drought)?</t>
+  </si>
+  <si>
+    <r>
+      <t>Over the past 4 years, has the $ amount of financing that can be mobilized through sovereign risk financing instruments increased?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Please provide numbers when available</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Since the adoption of the DRM legal framework: 
+(1) have DRM policy instruments (e.g., DRM strategies or policies) been officially approved? 
+(2)  have DRM-related regulations (e.g., rules on the structure or functions of the DRM agency) been officially approved? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">If yes, please specify which policy document(s) and/or regulation(s). </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Is there a reporting or monitoring mechanism to track progress toward DRM and/or CCA targets included in the National Development Strategies?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> If yes, please report those progress</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do key fiscal policy documents (e.g., the medium-term fiscal framework or fiscal risk statements) include quantified assessments of disaster risks? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>If yes, please specify which document(s).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Are there sovereign risk financing instruments (e.g., disaster or emergency funds, contingent loans, insurance or other risk transfer mechanisms) in place to manage the financial impact of disasters and climate-related shocks? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">If yes, please list them. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,6 +675,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1038,7 +1105,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1237,233 +1304,227 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -1518,7 +1579,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$D$2</c:f>
+              <c:f>'Summary (to be hidden)'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1539,7 +1600,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Summary!$B$3:$C$14</c:f>
+              <c:f>'Summary (to be hidden)'!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1550,7 +1611,7 @@
                     <c:v>Mainstreaming DRM into national and sectoral development plans</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Risk Identification</c:v>
+                    <c:v>Risk identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Territorial and urban planning</c:v>
@@ -1562,22 +1623,22 @@
                     <c:v>Sector-specific risk reduction measures</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Early Warning Systems (EWS)</c:v>
+                    <c:v>Early warning systems</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Emergency Preparedness and Response (EP&amp;R)</c:v>
+                    <c:v>Emergency preparedness and response</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Adaptive Social Protection (ASP)</c:v>
+                    <c:v>Adaptive social protection</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Fiscal risk management</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Disaster Risk Financing (DRF) strategies and instruments</c:v>
+                    <c:v>DRF strategies and instruments</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Resilient Reconstruction</c:v>
+                    <c:v>Resilient reconstruction</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1623,12 +1684,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$D$3:$D$14</c:f>
+              <c:f>'Summary (to be hidden)'!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1637,16 +1698,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1677,7 +1738,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$E$2</c:f>
+              <c:f>'Summary (to be hidden)'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1698,7 +1759,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Summary!$B$3:$C$14</c:f>
+              <c:f>'Summary (to be hidden)'!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1709,7 +1770,7 @@
                     <c:v>Mainstreaming DRM into national and sectoral development plans</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Risk Identification</c:v>
+                    <c:v>Risk identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Territorial and urban planning</c:v>
@@ -1721,22 +1782,22 @@
                     <c:v>Sector-specific risk reduction measures</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Early Warning Systems (EWS)</c:v>
+                    <c:v>Early warning systems</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Emergency Preparedness and Response (EP&amp;R)</c:v>
+                    <c:v>Emergency preparedness and response</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Adaptive Social Protection (ASP)</c:v>
+                    <c:v>Adaptive social protection</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Fiscal risk management</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Disaster Risk Financing (DRF) strategies and instruments</c:v>
+                    <c:v>DRF strategies and instruments</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Resilient Reconstruction</c:v>
+                    <c:v>Resilient reconstruction</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1782,7 +1843,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$E$3:$E$14</c:f>
+              <c:f>'Summary (to be hidden)'!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1793,16 +1854,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1836,7 +1897,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$F$2</c:f>
+              <c:f>'Summary (to be hidden)'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1857,7 +1918,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Summary!$B$3:$C$14</c:f>
+              <c:f>'Summary (to be hidden)'!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -1868,7 +1929,7 @@
                     <c:v>Mainstreaming DRM into national and sectoral development plans</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Risk Identification</c:v>
+                    <c:v>Risk identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Territorial and urban planning</c:v>
@@ -1880,22 +1941,22 @@
                     <c:v>Sector-specific risk reduction measures</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Early Warning Systems (EWS)</c:v>
+                    <c:v>Early warning systems</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Emergency Preparedness and Response (EP&amp;R)</c:v>
+                    <c:v>Emergency preparedness and response</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Adaptive Social Protection (ASP)</c:v>
+                    <c:v>Adaptive social protection</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Fiscal risk management</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Disaster Risk Financing (DRF) strategies and instruments</c:v>
+                    <c:v>DRF strategies and instruments</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Resilient Reconstruction</c:v>
+                    <c:v>Resilient reconstruction</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1941,33 +2002,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$F$3:$F$14</c:f>
+              <c:f>'Summary (to be hidden)'!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1995,7 +2056,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$G$2</c:f>
+              <c:f>'Summary (to be hidden)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2016,7 +2077,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Summary!$B$3:$C$14</c:f>
+              <c:f>'Summary (to be hidden)'!$B$3:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="12"/>
                 <c:lvl>
@@ -2027,7 +2088,7 @@
                     <c:v>Mainstreaming DRM into national and sectoral development plans</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Risk Identification</c:v>
+                    <c:v>Risk identification</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>Territorial and urban planning</c:v>
@@ -2039,22 +2100,22 @@
                     <c:v>Sector-specific risk reduction measures</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Early Warning Systems (EWS)</c:v>
+                    <c:v>Early warning systems</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Emergency Preparedness and Response (EP&amp;R)</c:v>
+                    <c:v>Emergency preparedness and response</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Adaptive Social Protection (ASP)</c:v>
+                    <c:v>Adaptive social protection</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Fiscal risk management</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Disaster Risk Financing (DRF) strategies and instruments</c:v>
+                    <c:v>DRF strategies and instruments</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Resilient Reconstruction</c:v>
+                    <c:v>Resilient reconstruction</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2100,7 +2161,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$G$3:$G$14</c:f>
+              <c:f>'Summary (to be hidden)'!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2108,25 +2169,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3267,7 +3328,7 @@
   <dimension ref="B2:AU50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3289,53 +3350,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:47" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="141" t="s">
-        <v>101</v>
+      <c r="B2" s="68" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:47" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="B4" s="143" t="s">
-        <v>99</v>
+      <c r="B4" s="70" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="144" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="144"/>
-      <c r="D6" s="144"/>
-      <c r="E6" s="145" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="145"/>
+      <c r="B6" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="78"/>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="146" t="str">
-        <f>_xlfn.TEXTJOIN(";",FALSE,Summary!I2:I14)</f>
-        <v>Pillar,Subpillar,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0;Risk Identification,Risk Identification,0,0,0,0;Risk Reduction,Territorial and urban planning,0,0,0,0;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0,0,0,0;Preparedness,Early Warning Systems (EWS),0,0,0,0;Preparedness,Emergency Preparedness and Response (EP&amp;R),0,0,0,0;Preparedness,Adaptive Social Protection (ASP),0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,Disaster Risk Financing (DRF) strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient Reconstruction,0,0,0,0</v>
+        <v>87</v>
+      </c>
+      <c r="E7" s="71" t="str">
+        <f>_xlfn.TEXTJOIN(";",FALSE,'Summary (to be hidden)'!I2:I14)</f>
+        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,1,0,1,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1;Risk Identification,Risk identification,0,0.5,0,1;Risk Reduction,Territorial and urban planning,1,1,1,1;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0.875,0.5,0.5,1;Preparedness,Early warning systems,1,0,1,1;Preparedness,Emergency preparedness and response,0,0,1,1;Preparedness,Adaptive social protection,0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,DRF strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
       </c>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="E9" s="67">
         <f>64-(COUNTIF('Diagnostic Questions'!D12:K50,"YES")+COUNTIF('Diagnostic Questions'!D12:K50,"NO"))</f>
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:47" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="142" t="s">
-        <v>82</v>
+      <c r="B10" s="69" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:47" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3344,24 +3405,24 @@
         <v>0</v>
       </c>
       <c r="C12" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="129" t="s">
+      <c r="E12" s="103"/>
+      <c r="F12" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="103"/>
+      <c r="H12" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="129" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="131"/>
-      <c r="H12" s="129" t="s">
+      <c r="I12" s="103"/>
+      <c r="J12" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="131"/>
-      <c r="J12" s="129" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" s="130"/>
+      <c r="K12" s="102"/>
       <c r="L12" s="33"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -3399,55 +3460,63 @@
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
     </row>
-    <row r="13" spans="2:47" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="68" t="s">
+    <row r="13" spans="2:47" s="1" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="D13" s="104" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="105"/>
+      <c r="F13" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="125" t="s">
+      <c r="G13" s="105"/>
+      <c r="H13" s="144" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="106"/>
+      <c r="J13" s="99" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="100"/>
+      <c r="L13" s="25"/>
+    </row>
+    <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="73"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="132"/>
-      <c r="F13" s="125" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="132"/>
-      <c r="H13" s="127" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="133"/>
-      <c r="J13" s="127" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="128"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="69"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="66"/>
+      <c r="E14" s="66" t="s">
+        <v>89</v>
+      </c>
       <c r="F14" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H14" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="J14" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="L14" s="25"/>
     </row>
     <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="69"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="140"/>
       <c r="D15" s="44"/>
       <c r="E15" s="48"/>
       <c r="F15" s="44"/>
@@ -3455,31 +3524,37 @@
       <c r="H15" s="46"/>
       <c r="I15" s="48"/>
       <c r="J15" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="18"/>
+        <v>62</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="L15" s="25"/>
     </row>
     <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="69"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="140"/>
       <c r="D16" s="44"/>
       <c r="E16" s="48"/>
       <c r="F16" s="44"/>
       <c r="G16" s="48"/>
       <c r="H16" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="J16" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" s="50"/>
+        <v>63</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="L16" s="25"/>
     </row>
     <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="69"/>
-      <c r="C17" s="74"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="45"/>
       <c r="E17" s="48"/>
       <c r="F17" s="45"/>
@@ -3491,106 +3566,122 @@
       <c r="L17" s="25"/>
     </row>
     <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="69"/>
-      <c r="C18" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="116" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="117"/>
-      <c r="H18" s="119" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="120"/>
-      <c r="J18" s="116" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="121"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="115"/>
+      <c r="F18" s="116" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="115"/>
+      <c r="H18" s="116" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="117"/>
+      <c r="J18" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="108"/>
       <c r="L18" s="34"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="70"/>
-      <c r="C19" s="82"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="76"/>
       <c r="D19" s="27" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>96</v>
+      </c>
       <c r="H19" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="J19" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="L19" s="35"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="108" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="114" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="115"/>
-      <c r="F20" s="114" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="115"/>
-      <c r="H20" s="114" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" s="115"/>
-      <c r="J20" s="114" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="124"/>
+      <c r="B20" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="109" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="110"/>
+      <c r="F20" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="110"/>
+      <c r="H20" s="109" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="110"/>
+      <c r="J20" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="111"/>
       <c r="L20" s="25"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="112"/>
-      <c r="C21" s="109"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="F21" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="J21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="L21" s="25"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="113"/>
-      <c r="C22" s="110"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="14"/>
       <c r="E22" s="58"/>
       <c r="F22" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="H22" s="52"/>
       <c r="I22" s="58"/>
       <c r="J22" s="52"/>
@@ -3598,54 +3689,62 @@
       <c r="L22" s="25"/>
     </row>
     <row r="23" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="122" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="87"/>
-      <c r="F23" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="87"/>
-      <c r="H23" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="87"/>
-      <c r="J23" s="125" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="126"/>
+      <c r="B23" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="114"/>
+      <c r="F23" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="114"/>
+      <c r="H23" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="114"/>
+      <c r="J23" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="112"/>
       <c r="L23" s="25"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="69"/>
-      <c r="C24" s="81"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F24" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="H24" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="J24" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="K24" s="18"/>
+        <v>66</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="L24" s="25"/>
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="69"/>
-      <c r="C25" s="123"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="87"/>
       <c r="D25" s="45"/>
       <c r="E25" s="48"/>
       <c r="F25" s="45"/>
@@ -3653,58 +3752,64 @@
       <c r="H25" s="45"/>
       <c r="I25" s="48"/>
       <c r="J25" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="K25" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>89</v>
+      </c>
       <c r="L25" s="25"/>
     </row>
     <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="69"/>
-      <c r="C26" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="84"/>
-      <c r="F26" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="84"/>
-      <c r="H26" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="84"/>
-      <c r="J26" s="75" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" s="77"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="95"/>
+      <c r="F26" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="95"/>
+      <c r="H26" s="94" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="95"/>
+      <c r="J26" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="143"/>
       <c r="L26" s="25"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="69"/>
-      <c r="C27" s="81"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="96"/>
       <c r="D27" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="F27" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H27" s="26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="28" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="25"/>
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="69"/>
-      <c r="C28" s="123"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="45"/>
       <c r="E28" s="48"/>
       <c r="F28" s="45"/>
@@ -3712,64 +3817,74 @@
       <c r="H28" s="45"/>
       <c r="I28" s="48"/>
       <c r="J28" s="29" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="K28" s="23"/>
       <c r="L28" s="25"/>
     </row>
     <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="69"/>
-      <c r="C29" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="75" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="85" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="85"/>
-      <c r="H29" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="I29" s="76"/>
-      <c r="J29" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="77"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="142"/>
+      <c r="F29" s="118" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="118"/>
+      <c r="H29" s="97" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" s="142"/>
+      <c r="J29" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="143"/>
       <c r="L29" s="25"/>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
-      <c r="C30" s="81"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="96"/>
       <c r="D30" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F30" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="H30" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="J30" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="K30" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="L30" s="25"/>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="69"/>
-      <c r="C31" s="81"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="96"/>
       <c r="D31" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F31" s="53"/>
       <c r="G31" s="48"/>
       <c r="H31" s="42"/>
@@ -3780,12 +3895,14 @@
       <c r="M31" s="4"/>
     </row>
     <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="69"/>
-      <c r="C32" s="81"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="96"/>
       <c r="D32" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="F32" s="53"/>
       <c r="G32" s="48"/>
       <c r="H32" s="42"/>
@@ -3796,12 +3913,14 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="69"/>
-      <c r="C33" s="81"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="96"/>
       <c r="D33" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="22"/>
+        <v>65</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="F33" s="53"/>
       <c r="G33" s="48"/>
       <c r="H33" s="43"/>
@@ -3812,311 +3931,339 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="69"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="97"/>
-      <c r="F34" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="76"/>
-      <c r="H34" s="85" t="s">
-        <v>37</v>
-      </c>
-      <c r="I34" s="85"/>
-      <c r="J34" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="K34" s="98"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="97" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="98"/>
+      <c r="F34" s="97" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" s="142"/>
+      <c r="H34" s="118" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="118"/>
+      <c r="J34" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="119"/>
       <c r="L34" s="25"/>
     </row>
     <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="69"/>
-      <c r="C35" s="81"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="96"/>
       <c r="D35" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="F35" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H35" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="J35" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="K35" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="L35" s="25"/>
     </row>
     <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="70"/>
-      <c r="C36" s="82"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="76"/>
       <c r="D36" s="54"/>
       <c r="E36" s="61"/>
       <c r="F36" s="54"/>
       <c r="G36" s="65"/>
       <c r="H36" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="J36" s="54"/>
       <c r="K36" s="62"/>
       <c r="L36" s="25"/>
     </row>
     <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="111" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="108" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="79"/>
-      <c r="F37" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" s="79"/>
-      <c r="H37" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="I37" s="79"/>
-      <c r="J37" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="K37" s="99"/>
+      <c r="B37" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="120" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="125"/>
+      <c r="F37" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="125"/>
+      <c r="H37" s="120" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="125"/>
+      <c r="J37" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="121"/>
       <c r="L37" s="36"/>
     </row>
     <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="112"/>
-      <c r="C38" s="134"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="22"/>
+        <v>7</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="F38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="22"/>
+        <v>7</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>96</v>
+      </c>
       <c r="H38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="22"/>
+        <v>7</v>
+      </c>
+      <c r="I38" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="J38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K38" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="L38" s="36"/>
     </row>
     <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="112"/>
-      <c r="C39" s="135" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="101"/>
-      <c r="F39" s="100" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="101"/>
-      <c r="H39" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I39" s="107"/>
-      <c r="J39" s="102" t="s">
-        <v>47</v>
-      </c>
-      <c r="K39" s="103"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="124" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="123"/>
+      <c r="F39" s="122" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="123"/>
+      <c r="H39" s="129" t="s">
+        <v>103</v>
+      </c>
+      <c r="I39" s="130"/>
+      <c r="J39" s="124" t="s">
+        <v>38</v>
+      </c>
+      <c r="K39" s="126"/>
       <c r="L39" s="1"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="112"/>
-      <c r="C40" s="109"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="F40" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H40" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="J40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40" s="18"/>
+        <v>7</v>
+      </c>
+      <c r="K40" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="L40" s="1"/>
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="112"/>
-      <c r="C41" s="134"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="21"/>
       <c r="E41" s="57"/>
       <c r="F41" s="21"/>
       <c r="G41" s="57"/>
       <c r="H41" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="22"/>
+        <v>62</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="J41" s="21"/>
       <c r="K41" s="64"/>
       <c r="L41" s="1"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="112"/>
-      <c r="C42" s="135" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="101"/>
-      <c r="F42" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="101"/>
-      <c r="H42" s="105" t="s">
-        <v>51</v>
-      </c>
-      <c r="I42" s="105"/>
-      <c r="J42" s="100" t="s">
-        <v>52</v>
-      </c>
-      <c r="K42" s="104"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="123"/>
+      <c r="F42" s="122" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" s="123"/>
+      <c r="H42" s="128" t="s">
+        <v>104</v>
+      </c>
+      <c r="I42" s="128"/>
+      <c r="J42" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="K42" s="127"/>
       <c r="L42" s="25"/>
     </row>
     <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="113"/>
-      <c r="C43" s="110"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="85"/>
       <c r="D43" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G43" s="19"/>
       <c r="H43" s="17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I43" s="19"/>
       <c r="J43" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K43" s="20"/>
       <c r="L43" s="25"/>
     </row>
     <row r="44" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="122" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="87"/>
-      <c r="F44" s="86" t="s">
-        <v>56</v>
-      </c>
-      <c r="G44" s="87"/>
-      <c r="H44" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="I44" s="87"/>
-      <c r="J44" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="K44" s="93"/>
+      <c r="B44" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="114"/>
+      <c r="F44" s="113" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="114"/>
+      <c r="H44" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="114"/>
+      <c r="J44" s="113" t="s">
+        <v>47</v>
+      </c>
+      <c r="K44" s="133"/>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="69"/>
-      <c r="C45" s="123"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="87"/>
       <c r="D45" s="29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I45" s="22"/>
       <c r="J45" s="29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K45" s="23"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="69"/>
-      <c r="C46" s="138" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="88"/>
-      <c r="F46" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="G46" s="92"/>
-      <c r="H46" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="I46" s="88"/>
-      <c r="J46" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="K46" s="94"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="137"/>
+      <c r="F46" s="131" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="132"/>
+      <c r="H46" s="137" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="137"/>
+      <c r="J46" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="K46" s="134"/>
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="69"/>
-      <c r="C47" s="139"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="92"/>
       <c r="D47" s="26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="28" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I47" s="11"/>
       <c r="J47" s="26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K47" s="18"/>
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="70"/>
-      <c r="C48" s="140"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="93"/>
       <c r="D48" s="54"/>
       <c r="E48" s="61"/>
       <c r="F48" s="32" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="56"/>
@@ -4126,113 +4273,53 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="111" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="136" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="79"/>
-      <c r="F49" s="89" t="s">
-        <v>66</v>
-      </c>
-      <c r="G49" s="90"/>
-      <c r="H49" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="I49" s="79"/>
-      <c r="J49" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="K49" s="96"/>
+      <c r="B49" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="120" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="125"/>
+      <c r="F49" s="120" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" s="125"/>
+      <c r="H49" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="125"/>
+      <c r="J49" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" s="136"/>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="113"/>
-      <c r="C50" s="137"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="89"/>
       <c r="D50" s="14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E50" s="19"/>
       <c r="F50" s="14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I50" s="19"/>
       <c r="J50" s="14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K50" s="20"/>
       <c r="L50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H44:I44"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="C13:C17"/>
     <mergeCell ref="D29:E29"/>
@@ -4249,8 +4336,68 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K27:K28 G14 E14 E19 G19 I19 K19 I16 G21:G22 K14:K16 E21 I21 K21 I24 G24 E24 E27 G27 G30 E35 I35:I36 G40 E40 K35 K40 E47 I47 E30:E33 G35 I38 K38 G38 E38 I40:I41 K43 I43 G43 E43 E45 E50 G50 G47:G48 I50 K50 K45 I45 G45 I30 K30 I27 K24:K25 I14 K47" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
@@ -4273,8 +4420,8 @@
   </sheetPr>
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4282,45 +4429,45 @@
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="40" t="s">
+      <c r="G2" s="40" t="s">
         <v>3</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>4</v>
       </c>
       <c r="I2" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B2:G2)</f>
-        <v>Pillar,Subpillar,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers</v>
+        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="39" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D3" s="39">
         <f>IF('Diagnostic Questions'!E14="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f>IF('Diagnostic Questions'!G14="Yes",1,0)</f>
@@ -4328,7 +4475,7 @@
       </c>
       <c r="F3" s="39">
         <f>0.5*IF('Diagnostic Questions'!I14="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I16="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="39">
         <f>ROUND(0.3333*IF('Diagnostic Questions'!K14="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K15="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K16="Yes",1,0),2)</f>
@@ -4336,15 +4483,15 @@
       </c>
       <c r="I3" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B3:G3)</f>
-        <v>Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0</v>
+        <v>Legal and Institutional DRM Framework,DRM policies and institutions,1,0,1,0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="39" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D4" s="39">
         <f>IF('Diagnostic Questions'!E19="Yes",1,0)</f>
@@ -4356,23 +4503,23 @@
       </c>
       <c r="F4" s="39">
         <f>IF('Diagnostic Questions'!I19="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="39">
         <f>IF('Diagnostic Questions'!K19="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B4:G4)</f>
-        <v>Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0</v>
+        <v>Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D5" s="39">
         <f>IF('Diagnostic Questions'!E21="Yes",1,0)</f>
@@ -4380,7 +4527,7 @@
       </c>
       <c r="E5" s="39">
         <f>0.5*IF('Diagnostic Questions'!G21="Yes",1,0) + 0.5*IF('Diagnostic Questions'!G22="Yes",1,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="39">
         <f>IF('Diagnostic Questions'!I21="Yes",1,0)</f>
@@ -4388,47 +4535,47 @@
       </c>
       <c r="G5" s="39">
         <f>IF('Diagnostic Questions'!K21="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I14" si="0">_xlfn.TEXTJOIN(",",FALSE,B5:G5)</f>
-        <v>Risk Identification,Risk Identification,0,0,0,0</v>
+        <v>Risk Identification,Risk identification,0,0.5,0,1</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D6" s="39">
         <f>IF('Diagnostic Questions'!E24="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="39">
         <f>IF('Diagnostic Questions'!G24="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="39">
         <f>IF('Diagnostic Questions'!I24="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="39">
         <f>0.5*IF('Diagnostic Questions'!K24="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K25="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>Risk Reduction,Territorial and urban planning,0,0,0,0</v>
+        <v>Risk Reduction,Territorial and urban planning,1,1,1,1</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="39" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D7" s="39">
         <f>IF('Diagnostic Questions'!E27="Yes",1,0)</f>
@@ -4453,42 +4600,42 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="39" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D8" s="39">
         <f>0.5*(0.25*IF('Diagnostic Questions'!E30="Yes",1,0)+0.25*IF('Diagnostic Questions'!E31="Yes",1,0)+0.25*IF('Diagnostic Questions'!E32="Yes",1,0)+0.25*IF('Diagnostic Questions'!E33="Yes",1,0))+0.5*IF('Diagnostic Questions'!E35="Yes",1,0)</f>
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="E8" s="39">
         <f>0.5*IF('Diagnostic Questions'!G30="Yes",1,0)+0.5*IF('Diagnostic Questions'!G35="Yes",1,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="39">
         <f>0.5*IF('Diagnostic Questions'!I30="Yes",1,0)+0.5*(0.5*IF('Diagnostic Questions'!I35="Yes",1,0)+0.5*IF('Diagnostic Questions'!I36="Yes",1,0))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="39">
         <f>0.5*IF('Diagnostic Questions'!K30="Yes",1,0)+0.5*IF('Diagnostic Questions'!K35="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>Risk Reduction,Sector-specific risk reduction measures,0,0,0,0</v>
+        <v>Risk Reduction,Sector-specific risk reduction measures,0.875,0.5,0.5,1</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="39" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D9" s="39">
         <f>IF('Diagnostic Questions'!E38="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="39">
         <f>IF('Diagnostic Questions'!G38="Yes",1,0)</f>
@@ -4496,23 +4643,23 @@
       </c>
       <c r="F9" s="39">
         <f>IF('Diagnostic Questions'!I38="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="39">
         <f>IF('Diagnostic Questions'!K38="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>Preparedness,Early Warning Systems (EWS),0,0,0,0</v>
+        <v>Preparedness,Early warning systems,1,0,1,1</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="39" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D10" s="39">
         <f>IF('Diagnostic Questions'!E40="Yes",1,0)</f>
@@ -4524,23 +4671,23 @@
       </c>
       <c r="F10" s="39">
         <f>0.5*IF('Diagnostic Questions'!I40="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I41="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="39">
         <f>IF('Diagnostic Questions'!K40="Yes",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>Preparedness,Emergency Preparedness and Response (EP&amp;R),0,0,0,0</v>
+        <v>Preparedness,Emergency preparedness and response,0,0,1,1</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="39" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D11" s="39">
         <f>IF('Diagnostic Questions'!E43="Yes",1,0)</f>
@@ -4560,15 +4707,15 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>Preparedness,Adaptive Social Protection (ASP),0,0,0,0</v>
+        <v>Preparedness,Adaptive social protection,0,0,0,0</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D12" s="39">
         <f>IF('Diagnostic Questions'!E45="Yes",1,0)</f>
@@ -4593,10 +4740,10 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="39" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D13" s="39">
         <f>IF('Diagnostic Questions'!E47="Yes",1,0)</f>
@@ -4616,15 +4763,15 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
-        <v>Financial Protection,Disaster Risk Financing (DRF) strategies and instruments,0,0,0,0</v>
+        <v>Financial Protection,DRF strategies and instruments,0,0,0,0</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="39" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14" s="39">
         <f>IF('Diagnostic Questions'!E50="Yes",1,0)</f>
@@ -4644,7 +4791,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
-        <v>Resilient Reconstruction,Resilient Reconstruction,0,0,0,0</v>
+        <v>Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Move contextual info to top of main content
Relocated the disaster risk management contextual information to the top of the main content area for improved visibility and user experience. Updated the layout in app.py accordingly.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1609" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDDBB970-0B64-4DE6-B91C-21E2C866740E}"/>
+  <xr:revisionPtr revIDLastSave="1640" documentId="8_{897DEB52-8293-498E-AAF6-D0CE94892166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598D8B80-4FD8-4E53-9B77-942B9EE6EEF2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="30612" yWindow="4248" windowWidth="23256" windowHeight="12456" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagnostic Questions" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Have guidelines or regulations to conduct post-disaster damage and needs assessments been developed and approved?</t>
   </si>
   <si>
-    <t>Do laws and regulations clearly define institutional responsibilities and mandates for producing, acquiring, and managing risk information (e.g., hazard information, vulnerability assessments, risk profiles, historical disaster databases)?</t>
-  </si>
-  <si>
     <t>Do at least half of the essential government entities use existing risk information to inform their sectoral planning processes?</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
     <t xml:space="preserve">Do official guidelines exist defining disaster and climate risk screening methodologies for new public investment projects? </t>
   </si>
   <si>
-    <t>Do the legal framework and institutional arrangements for water supply and sanitation in urban areas take flood risk into account?</t>
-  </si>
-  <si>
     <t>Are there legal and institutional arrangements for integrated water resources management (IWRM) that explicitly incorporate flood and drought risk considerations?</t>
   </si>
   <si>
@@ -406,83 +400,37 @@
     <t>During the most recent disaster or climate-related shock, was support promptly provided to the population through social‐protection programs?  (e.g., cash transfers in the case of drought)?</t>
   </si>
   <si>
-    <r>
-      <t>Over the past 4 years, has the $ amount of financing that can be mobilized through sovereign risk financing instruments increased?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Please provide numbers when available</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Since the adoption of the DRM legal framework: 
+    <t>sheet password is 1234</t>
+  </si>
+  <si>
+    <t>Since the adoption of the DRM legal framework: 
 (1) have DRM policy instruments (e.g., DRM strategies or policies) been officially approved? 
-(2)  have DRM-related regulations (e.g., rules on the structure or functions of the DRM agency) been officially approved? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">If yes, please specify which policy document(s) and/or regulation(s). </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Is there a reporting or monitoring mechanism to track progress toward DRM and/or CCA targets included in the National Development Strategies?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> If yes, please report those progress</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Do key fiscal policy documents (e.g., the medium-term fiscal framework or fiscal risk statements) include quantified assessments of disaster risks? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>If yes, please specify which document(s).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Are there sovereign risk financing instruments (e.g., disaster or emergency funds, contingent loans, insurance or other risk transfer mechanisms) in place to manage the financial impact of disasters and climate-related shocks? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">If yes, please list them. </t>
-    </r>
+(2)  have DRM-related regulations (e.g., rules on the structure or functions of the DRM agency) been officially approved?</t>
+  </si>
+  <si>
+    <t>Is there a reporting or monitoring mechanism to track progress toward DRM and/or CCA targets included in the National Development Strategies?</t>
+  </si>
+  <si>
+    <t>Do key fiscal policy documents (e.g., the medium-term fiscal framework or fiscal risk statements) include quantified assessments of disaster risks?</t>
+  </si>
+  <si>
+    <t>Over the past 4 years, has the $ amount of financing that can be mobilized through sovereign risk financing instruments increased?</t>
+  </si>
+  <si>
+    <t>Are there sovereign risk financing instruments (e.g., disaster or emergency funds, contingent loans, insurance or other risk transfer mechanisms) in place to manage the financial impact of disasters and climate-related shocks?</t>
+  </si>
+  <si>
+    <t>Do laws and regulations clearly define institutional responsibilities and mandates for producing, acquiring, and managing geospatial information, including risk information (e.g., hazard information, vulnerability assessments, risk profiles, historical disaster databases)?</t>
+  </si>
+  <si>
+    <t>Are there legal and institutional arrangements for water supply and sanitation in urban areas that take flood risk into account?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,12 +623,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1105,7 +1047,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1123,84 +1065,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1212,94 +1082,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1308,222 +1094,504 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1704,7 +1772,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.875</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1848,7 +1916,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2022,7 +2090,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3327,8 +3395,8 @@
   </sheetPr>
   <dimension ref="B2:AU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3337,93 +3405,93 @@
     <col min="2" max="2" width="22.5546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="21.109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="41.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
     <col min="6" max="6" width="54.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="7" customWidth="1"/>
     <col min="8" max="8" width="65" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" style="24" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="7" customWidth="1"/>
     <col min="10" max="10" width="55.5546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" style="7" customWidth="1"/>
     <col min="12" max="12" width="38.88671875" customWidth="1"/>
     <col min="13" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="47" width="9.109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:47" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="68" t="s">
-        <v>83</v>
+      <c r="B2" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:47" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="B4" s="70" t="s">
-        <v>81</v>
+      <c r="B4" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="77" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="78"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="71" t="str">
+        <v>86</v>
+      </c>
+      <c r="E7" s="19" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,'Summary (to be hidden)'!I2:I14)</f>
-        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,1,0,1,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1;Risk Identification,Risk identification,0,0.5,0,1;Risk Reduction,Territorial and urban planning,1,1,1,1;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0.875,0.5,0.5,1;Preparedness,Early warning systems,1,0,1,1;Preparedness,Emergency preparedness and response,0,0,1,1;Preparedness,Adaptive social protection,0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,DRF strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
+        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,1,1,1,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1;Risk Identification,Risk identification,0,0.5,0,1;Risk Reduction,Territorial and urban planning,1,1,1,1;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0.8,0.5,1,1;Preparedness,Early warning systems,1,0,1,1;Preparedness,Emergency preparedness and response,0,0,1,1;Preparedness,Adaptive social protection,0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,DRF strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
       </c>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="67">
+        <v>83</v>
+      </c>
+      <c r="E9" s="15">
         <f>64-(COUNTIF('Diagnostic Questions'!D12:K50,"YES")+COUNTIF('Diagnostic Questions'!D12:K50,"NO"))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:47" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
-        <v>68</v>
+      <c r="B10" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:47" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:47" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="101" t="s">
+      <c r="C12" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="101" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="103"/>
-      <c r="H12" s="101" t="s">
+      <c r="E12" s="26"/>
+      <c r="F12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="26"/>
+      <c r="H12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="103"/>
-      <c r="J12" s="101" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="102"/>
-      <c r="L12" s="33"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -3461,865 +3529,928 @@
       <c r="AU12" s="2"/>
     </row>
     <row r="13" spans="2:47" s="1" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="138" t="s">
+      <c r="C13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="105"/>
-      <c r="F13" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="144" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" s="106"/>
-      <c r="J13" s="99" t="s">
+      <c r="K13" s="35"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="58"/>
+      <c r="J18" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="59"/>
+      <c r="L18" s="10"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="60"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="68"/>
+      <c r="F20" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="68"/>
+      <c r="H20" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="68"/>
+      <c r="J20" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="69"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="80"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="K13" s="100"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="73"/>
-      <c r="C14" s="139"/>
-      <c r="D14" s="41" t="s">
+      <c r="E23" s="84"/>
+      <c r="F23" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="84"/>
+      <c r="H23" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="84"/>
+      <c r="J23" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="85"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="36"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="26" t="s">
+      <c r="E24" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="26" t="s">
+      <c r="G24" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="36"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" s="26" t="s">
+      <c r="K25" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="36"/>
+      <c r="C26" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="91"/>
+      <c r="F26" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="91"/>
+      <c r="H26" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="91"/>
+      <c r="J26" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="93"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="36"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="41"/>
+      <c r="J27" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="42"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="36"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="L14" s="25"/>
-    </row>
-    <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="73"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="73"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J16" s="49" t="s">
+      <c r="K28" s="89"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="36"/>
+      <c r="C29" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="95"/>
+      <c r="F29" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="96"/>
+      <c r="H29" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="95"/>
+      <c r="J29" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="93"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="36"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="L30" s="8"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="36"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" s="97"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="99"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="36"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="73"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="73"/>
-      <c r="C18" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="107" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="115"/>
-      <c r="F18" s="116" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="115"/>
-      <c r="H18" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="108"/>
-      <c r="L18" s="34"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="74"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="27" t="s">
+      <c r="E32" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="97"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="99"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="36"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" s="97"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="99"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="36"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="102"/>
+      <c r="F34" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="95"/>
+      <c r="H34" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="96"/>
+      <c r="J34" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="103"/>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="36"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="27" t="s">
+      <c r="E35" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="27" t="s">
+      <c r="G35" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="I35" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="27" t="s">
+      <c r="K35" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="60"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="107"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="109" t="s">
+        <v>61</v>
+      </c>
+      <c r="I36" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="106"/>
+      <c r="K36" s="110"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="111" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="112"/>
+      <c r="F37" s="111" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="112"/>
+      <c r="H37" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="112"/>
+      <c r="J37" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="113"/>
+      <c r="L37" s="12"/>
+    </row>
+    <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="70"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="L19" s="35"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="82" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="109" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="110"/>
-      <c r="F20" s="109" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="109" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="110"/>
-      <c r="J20" s="109" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="111"/>
-      <c r="L20" s="25"/>
-    </row>
-    <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="81"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="9" t="s">
+      <c r="E38" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="7" t="s">
+      <c r="G38" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="9" t="s">
+      <c r="I38" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="L21" s="25"/>
-    </row>
-    <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="80"/>
-      <c r="C22" s="85"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="25"/>
-    </row>
-    <row r="23" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="113" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="114"/>
-      <c r="F23" s="113" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="114"/>
-      <c r="H23" s="113" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="114"/>
-      <c r="J23" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="112"/>
-      <c r="L23" s="25"/>
-    </row>
-    <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="73"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="L24" s="25"/>
-    </row>
-    <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="73"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L25" s="25"/>
-    </row>
-    <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="73"/>
-      <c r="C26" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="94" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="95"/>
-      <c r="F26" s="94" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" s="95"/>
-      <c r="H26" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="95"/>
-      <c r="J26" s="97" t="s">
-        <v>23</v>
-      </c>
-      <c r="K26" s="143"/>
-      <c r="L26" s="25"/>
-    </row>
-    <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="73"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="25"/>
-    </row>
-    <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="73"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="23"/>
-      <c r="L28" s="25"/>
-    </row>
-    <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="73"/>
-      <c r="C29" s="75" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="142"/>
-      <c r="F29" s="118" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="118"/>
-      <c r="H29" s="97" t="s">
-        <v>58</v>
-      </c>
-      <c r="I29" s="142"/>
-      <c r="J29" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="K29" s="143"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="73"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="73"/>
-      <c r="C31" s="96"/>
-      <c r="D31" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31" s="53"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="73"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="53"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="73"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="73"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="97" t="s">
+      <c r="K38" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="70"/>
+      <c r="C39" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="117" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="118"/>
+      <c r="F39" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="118"/>
+      <c r="H39" s="120" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="98"/>
-      <c r="F34" s="97" t="s">
-        <v>102</v>
-      </c>
-      <c r="G34" s="142"/>
-      <c r="H34" s="118" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="118"/>
-      <c r="J34" s="97" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="119"/>
-      <c r="L34" s="25"/>
-    </row>
-    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H35" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J35" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="L35" s="25"/>
-    </row>
-    <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="74"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="J36" s="54"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="25"/>
-    </row>
-    <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="79" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="120" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="125"/>
-      <c r="F37" s="120" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="125"/>
-      <c r="H37" s="120" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="125"/>
-      <c r="J37" s="120" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" s="121"/>
-      <c r="L37" s="36"/>
-    </row>
-    <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="81"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="L38" s="36"/>
-    </row>
-    <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="81"/>
-      <c r="C39" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="124" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="123"/>
-      <c r="F39" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" s="123"/>
-      <c r="H39" s="129" t="s">
-        <v>103</v>
-      </c>
-      <c r="I39" s="130"/>
-      <c r="J39" s="124" t="s">
+      <c r="I39" s="121"/>
+      <c r="J39" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="K39" s="126"/>
+      <c r="K39" s="122"/>
       <c r="L39" s="1"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="81"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="13" t="s">
+      <c r="B40" s="70"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="13" t="s">
+      <c r="E40" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J40" s="8" t="s">
+      <c r="G40" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" s="123" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="18" t="s">
-        <v>89</v>
+      <c r="K40" s="42" t="s">
+        <v>88</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="81"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="J41" s="21"/>
-      <c r="K41" s="64"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="126"/>
+      <c r="F41" s="125"/>
+      <c r="G41" s="126"/>
+      <c r="H41" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="J41" s="125"/>
+      <c r="K41" s="127"/>
       <c r="L41" s="1"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="81"/>
-      <c r="C42" s="84" t="s">
+      <c r="B42" s="70"/>
+      <c r="C42" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="122" t="s">
+      <c r="D42" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="123"/>
-      <c r="F42" s="122" t="s">
+      <c r="E42" s="118"/>
+      <c r="F42" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="G42" s="123"/>
+      <c r="G42" s="118"/>
       <c r="H42" s="128" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I42" s="128"/>
-      <c r="J42" s="122" t="s">
+      <c r="J42" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="K42" s="127"/>
-      <c r="L42" s="25"/>
+      <c r="K42" s="129"/>
+      <c r="L42" s="8"/>
     </row>
     <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="80"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="16" t="s">
+      <c r="B43" s="75"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="16" t="s">
+      <c r="E43" s="63"/>
+      <c r="F43" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="17" t="s">
+      <c r="G43" s="63"/>
+      <c r="H43" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="16" t="s">
+      <c r="I43" s="63"/>
+      <c r="J43" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="K43" s="20"/>
-      <c r="L43" s="25"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="8"/>
     </row>
     <row r="44" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="113" t="s">
+      <c r="D44" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="114"/>
-      <c r="F44" s="113" t="s">
+      <c r="E44" s="84"/>
+      <c r="F44" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="G44" s="114"/>
-      <c r="H44" s="113" t="s">
+      <c r="G44" s="84"/>
+      <c r="H44" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="84"/>
+      <c r="J44" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="K44" s="132"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="36"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="100"/>
+      <c r="F45" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="100"/>
+      <c r="H45" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="100"/>
+      <c r="J45" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="89"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="36"/>
+      <c r="C46" s="133" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="I44" s="114"/>
-      <c r="J44" s="113" t="s">
-        <v>47</v>
-      </c>
-      <c r="K44" s="133"/>
-      <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="73"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="29" t="s">
+      <c r="E46" s="134"/>
+      <c r="F46" s="135" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="136"/>
+      <c r="H46" s="134" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="134"/>
+      <c r="J46" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="K46" s="137"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="36"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="29" t="s">
+      <c r="E47" s="41"/>
+      <c r="F47" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" s="41"/>
+      <c r="H47" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="22"/>
-      <c r="H45" s="29" t="s">
+      <c r="I47" s="41"/>
+      <c r="J47" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="29" t="s">
+      <c r="K47" s="42"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="60"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="G48" s="63"/>
+      <c r="H48" s="141"/>
+      <c r="I48" s="107"/>
+      <c r="J48" s="106"/>
+      <c r="K48" s="110"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="112"/>
+      <c r="F49" s="111" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" s="112"/>
+      <c r="H49" s="111" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="112"/>
+      <c r="J49" s="143" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" s="144"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="75"/>
+      <c r="C50" s="145"/>
+      <c r="D50" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="23"/>
-      <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="73"/>
-      <c r="C46" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="94" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" s="137"/>
-      <c r="F46" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="132"/>
-      <c r="H46" s="137" t="s">
-        <v>105</v>
-      </c>
-      <c r="I46" s="137"/>
-      <c r="J46" s="131" t="s">
-        <v>50</v>
-      </c>
-      <c r="K46" s="134"/>
-      <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="73"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="26" t="s">
+      <c r="E50" s="63"/>
+      <c r="F50" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="55" t="s">
+      <c r="G50" s="63"/>
+      <c r="H50" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="26" t="s">
+      <c r="I50" s="63"/>
+      <c r="J50" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="74"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="62"/>
-      <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="120" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="125"/>
-      <c r="F49" s="120" t="s">
-        <v>53</v>
-      </c>
-      <c r="G49" s="125"/>
-      <c r="H49" s="120" t="s">
-        <v>54</v>
-      </c>
-      <c r="I49" s="125"/>
-      <c r="J49" s="135" t="s">
-        <v>55</v>
-      </c>
-      <c r="K49" s="136"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="80"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="19"/>
-      <c r="F50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="19"/>
-      <c r="J50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="20"/>
+      <c r="K50" s="64"/>
       <c r="L50" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="qHxMlw49t7cqo6EtZn1JiBEwhCFMVlVf09HtocEiB3234myTQ3Iz4EJJRZvPPi8M/sZ/XjG+4AZMQVCjHtmYJw==" saltValue="ptowAI5jvPGgMLBWmqqr8w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="76">
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H44:I44"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="C13:C17"/>
     <mergeCell ref="D29:E29"/>
@@ -4336,66 +4467,6 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K27:K28 G14 E14 E19 G19 I19 K19 I16 G21:G22 K14:K16 E21 I21 K21 I24 G24 E24 E27 G27 G30 E35 I35:I36 G40 E40 K35 K40 E47 I47 E30:E33 G35 I38 K38 G38 E38 I40:I41 K43 I43 G43 E43 E45 E50 G50 G47:G48 I50 K50 K45 I45 G45 I30 K30 I27 K24:K25 I14 K47" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">
@@ -4418,10 +4489,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:I16"/>
+  <dimension ref="B2:I47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4435,22 +4506,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="str">
@@ -4459,53 +4530,53 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="39">
+      <c r="B3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="13">
         <f>IF('Diagnostic Questions'!E14="Yes",1,0)</f>
         <v>1</v>
       </c>
       <c r="E3">
         <f>IF('Diagnostic Questions'!G14="Yes",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="39">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
         <f>0.5*IF('Diagnostic Questions'!I14="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I16="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="13">
         <f>ROUND(0.3333*IF('Diagnostic Questions'!K14="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K15="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K16="Yes",1,0),2)</f>
         <v>0</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B3:G3)</f>
-        <v>Legal and Institutional DRM Framework,DRM policies and institutions,1,0,1,0</v>
+        <v>Legal and Institutional DRM Framework,DRM policies and institutions,1,1,1,0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="39">
+      <c r="B4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="13">
         <f>IF('Diagnostic Questions'!E19="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="13">
         <f>IF('Diagnostic Questions'!G19="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="13">
         <f>IF('Diagnostic Questions'!I19="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="13">
         <f>IF('Diagnostic Questions'!K19="Yes",1,0)</f>
         <v>1</v>
       </c>
@@ -4515,25 +4586,25 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="39">
+      <c r="B5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="13">
         <f>IF('Diagnostic Questions'!E21="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="13">
         <f>0.5*IF('Diagnostic Questions'!G21="Yes",1,0) + 0.5*IF('Diagnostic Questions'!G22="Yes",1,0)</f>
         <v>0.5</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="13">
         <f>IF('Diagnostic Questions'!I21="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="13">
         <f>IF('Diagnostic Questions'!K21="Yes",1,0)</f>
         <v>1</v>
       </c>
@@ -4543,25 +4614,25 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="39">
+      <c r="B6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="13">
         <f>IF('Diagnostic Questions'!E24="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="13">
         <f>IF('Diagnostic Questions'!G24="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="13">
         <f>IF('Diagnostic Questions'!I24="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="13">
         <f>0.5*IF('Diagnostic Questions'!K24="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K25="Yes",1,0)</f>
         <v>1</v>
       </c>
@@ -4571,25 +4642,25 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="39">
+      <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="13">
         <f>IF('Diagnostic Questions'!E27="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="13">
         <f>IF('Diagnostic Questions'!G27="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="13">
         <f>IF('Diagnostic Questions'!I27="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="13">
         <f>0.5*IF('Diagnostic Questions'!K27="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K28="Yes",1,0)</f>
         <v>0</v>
       </c>
@@ -4599,53 +4670,53 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="39">
-        <f>0.5*(0.25*IF('Diagnostic Questions'!E30="Yes",1,0)+0.25*IF('Diagnostic Questions'!E31="Yes",1,0)+0.25*IF('Diagnostic Questions'!E32="Yes",1,0)+0.25*IF('Diagnostic Questions'!E33="Yes",1,0))+0.5*IF('Diagnostic Questions'!E35="Yes",1,0)</f>
-        <v>0.875</v>
-      </c>
-      <c r="E8" s="39">
+      <c r="B8" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="13">
+        <f>0.2*IF('Diagnostic Questions'!E30="Yes",1,0)+0.2*IF('Diagnostic Questions'!E31="Yes",1,0)+0.2*IF('Diagnostic Questions'!E32="Yes",1,0)+0.2*IF('Diagnostic Questions'!E33="Yes",1,0)+0.2*IF('Diagnostic Questions'!E35="Yes",1,0)</f>
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="13">
         <f>0.5*IF('Diagnostic Questions'!G30="Yes",1,0)+0.5*IF('Diagnostic Questions'!G35="Yes",1,0)</f>
         <v>0.5</v>
       </c>
-      <c r="F8" s="39">
-        <f>0.5*IF('Diagnostic Questions'!I30="Yes",1,0)+0.5*(0.5*IF('Diagnostic Questions'!I35="Yes",1,0)+0.5*IF('Diagnostic Questions'!I36="Yes",1,0))</f>
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="39">
+      <c r="F8" s="13">
+        <f>ROUND(0.3333*IF('Diagnostic Questions'!I30="Yes",1,0)+0.3333*IF('Diagnostic Questions'!I35="Yes",1,0)+0.3333*IF('Diagnostic Questions'!I36="Yes",1,0),2)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
         <f>0.5*IF('Diagnostic Questions'!K30="Yes",1,0)+0.5*IF('Diagnostic Questions'!K35="Yes",1,0)</f>
         <v>1</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>Risk Reduction,Sector-specific risk reduction measures,0.875,0.5,0.5,1</v>
+        <v>Risk Reduction,Sector-specific risk reduction measures,0.8,0.5,1,1</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="39">
+      <c r="B9" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="13">
         <f>IF('Diagnostic Questions'!E38="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="13">
         <f>IF('Diagnostic Questions'!G38="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="13">
         <f>IF('Diagnostic Questions'!I38="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="13">
         <f>IF('Diagnostic Questions'!K38="Yes",1,0)</f>
         <v>1</v>
       </c>
@@ -4655,25 +4726,25 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="39">
+      <c r="B10" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="13">
         <f>IF('Diagnostic Questions'!E40="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="13">
         <f>IF('Diagnostic Questions'!G40="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="13">
         <f>0.5*IF('Diagnostic Questions'!I40="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I41="Yes",1,0)</f>
         <v>1</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="13">
         <f>IF('Diagnostic Questions'!K40="Yes",1,0)</f>
         <v>1</v>
       </c>
@@ -4683,25 +4754,25 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="39">
+      <c r="B11" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="13">
         <f>IF('Diagnostic Questions'!E43="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="13">
         <f>IF('Diagnostic Questions'!G43="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="13">
         <f>IF('Diagnostic Questions'!I43="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G11" s="13">
         <f>IF('Diagnostic Questions'!K43="Yes",1,0)</f>
         <v>0</v>
       </c>
@@ -4711,25 +4782,25 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="B12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="13">
         <f>IF('Diagnostic Questions'!E45="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="13">
         <f>IF('Diagnostic Questions'!G45="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="13">
         <f>IF('Diagnostic Questions'!I45="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="13">
         <f>IF('Diagnostic Questions'!K45="Yes",1,0)</f>
         <v>0</v>
       </c>
@@ -4739,25 +4810,25 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="39">
+      <c r="B13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="13">
         <f>IF('Diagnostic Questions'!E47="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="13">
         <f>0.5*IF('Diagnostic Questions'!G47="Yes",1,0)+0.5*IF('Diagnostic Questions'!G48="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="13">
         <f>IF('Diagnostic Questions'!I47="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="13">
         <f>IF('Diagnostic Questions'!K47="Yes",1,0)</f>
         <v>0</v>
       </c>
@@ -4767,25 +4838,25 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="39">
+      <c r="B14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="13">
         <f>IF('Diagnostic Questions'!E50="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="13">
         <f>IF('Diagnostic Questions'!G50="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="13">
         <f>IF('Diagnostic Questions'!I50="Yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="13">
         <f>IF('Diagnostic Questions'!K50="Yes",1,0)</f>
         <v>0</v>
       </c>
@@ -4796,6 +4867,14 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor results section layout and update template
Improved the layout of the assessment results section for better alignment and readability, consolidated and clarified interpretation text, and updated the DRM System Diagnostic Assessment template Excel file.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783161E0-90EF-4614-AEBE-8F830DC54AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B997EEB-7916-4D71-823D-9183477A5203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="4248" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diagnostic Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary (to be hidden)" sheetId="2" r:id="rId2"/>
+    <sheet name="DRM Diagnostic" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary (to be hidden)" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Thematic Area</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>DRF strategies and instruments</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
   </si>
   <si>
     <t>Resilient reconstruction</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Is there a legal framework (e.g., a DRM law or other instruments) defining distinct mandates for disaster risk reduction and emergency management?</t>
@@ -1317,12 +1311,232 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1341,10 +1555,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1353,18 +1563,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1373,10 +1571,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1389,207 +1583,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1943,22 +1937,20 @@
   </sheetPr>
   <dimension ref="B2:AU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="21.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="7" customWidth="1"/>
     <col min="6" max="6" width="54.5546875" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" style="7" customWidth="1"/>
     <col min="8" max="8" width="65" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="55.5546875" customWidth="1"/>
+    <col min="10" max="10" width="57.77734375" customWidth="1"/>
     <col min="11" max="11" width="9.5546875" style="7" customWidth="1"/>
     <col min="12" max="12" width="38.88671875" customWidth="1"/>
     <col min="13" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
@@ -1982,15 +1974,15 @@
       </c>
     </row>
     <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79" t="s">
+      <c r="C6" s="133"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="134"/>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
@@ -1998,7 +1990,7 @@
       </c>
       <c r="E7" s="19" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,'Summary (to be hidden)'!I2:I14)</f>
-        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,1,1,1,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1;Risk Identification,Risk identification,0,0.5,0,1;Risk Reduction,Territorial and urban planning,1,1,1,1;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0.8,0.5,1,1;Preparedness,Early warning systems,1,0,1,1;Preparedness,Emergency preparedness and response,0,0,1,1;Preparedness,Adaptive social protection,0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,DRF strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
+        <v>DRM Pillar,Thematic Area,Legal and institutional set up,Intermediary DRM outputs,Key DRM achievements,Policy enablers;Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0;Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0;Risk Identification,Risk identification,0,0,0,0;Risk Reduction,Territorial and urban planning,0,0,0,0;Risk Reduction,Public investment at the central level,0,0,0,0;Risk Reduction,Sector-specific risk reduction measures,0,0,0,0;Preparedness,Early warning systems,0,0,0,0;Preparedness,Emergency preparedness and response,0,0,0,0;Preparedness,Adaptive social protection,0,0,0,0;Financial Protection,Fiscal risk management,0,0,0,0;Financial Protection,DRF strategies and instruments,0,0,0,0;Resilient Reconstruction,Resilient reconstruction,0,0,0,0</v>
       </c>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.35">
@@ -2006,8 +1998,8 @@
         <v>83</v>
       </c>
       <c r="E9" s="15">
-        <f>64-(COUNTIF('Diagnostic Questions'!D12:K50,"YES")+COUNTIF('Diagnostic Questions'!D12:K50,"NO"))</f>
-        <v>20</v>
+        <f>64-(COUNTIF('DRM Diagnostic'!D12:K50,"YES")+COUNTIF('DRM Diagnostic'!D12:K50,"NO"))</f>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:47" ht="15.6" x14ac:dyDescent="0.3">
@@ -2023,22 +2015,22 @@
       <c r="C12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="104"/>
-      <c r="F12" s="102" t="s">
+      <c r="E12" s="129"/>
+      <c r="F12" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="104"/>
-      <c r="H12" s="102" t="s">
+      <c r="G12" s="129"/>
+      <c r="H12" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="104"/>
-      <c r="J12" s="102" t="s">
+      <c r="I12" s="129"/>
+      <c r="J12" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="103"/>
+      <c r="K12" s="128"/>
       <c r="L12" s="9"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -2080,59 +2072,51 @@
       <c r="B13" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="105" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="105" t="s">
+      <c r="D13" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="130"/>
+      <c r="F13" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="106"/>
-      <c r="H13" s="107" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="108"/>
-      <c r="J13" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="K13" s="101"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="132"/>
+      <c r="J13" s="125" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="126"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="74"/>
-      <c r="C14" s="141"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>88</v>
-      </c>
+      <c r="E14" s="24"/>
       <c r="F14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I14" s="26"/>
       <c r="J14" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="27" t="s">
-        <v>95</v>
-      </c>
+      <c r="K14" s="27"/>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="74"/>
-      <c r="C15" s="142"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="F15" s="28"/>
@@ -2142,14 +2126,12 @@
       <c r="J15" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K15" s="27" t="s">
-        <v>95</v>
-      </c>
+      <c r="K15" s="27"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="74"/>
-      <c r="C16" s="142"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
       <c r="F16" s="28"/>
@@ -2157,20 +2139,16 @@
       <c r="H16" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I16" s="26"/>
       <c r="J16" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="33" t="s">
-        <v>95</v>
-      </c>
+      <c r="K16" s="33"/>
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="74"/>
-      <c r="C17" s="143"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="34"/>
       <c r="E17" s="29"/>
       <c r="F17" s="34"/>
@@ -2183,123 +2161,105 @@
     </row>
     <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74"/>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="109" t="s">
+      <c r="D18" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="118" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118" t="s">
+      <c r="E18" s="119"/>
+      <c r="F18" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="119"/>
+      <c r="H18" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="119"/>
-      <c r="J18" s="109" t="s">
+      <c r="I18" s="121"/>
+      <c r="J18" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="110"/>
+      <c r="K18" s="111"/>
       <c r="L18" s="10"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="75"/>
-      <c r="C19" s="77"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="38" t="s">
-        <v>95</v>
-      </c>
+      <c r="E19" s="38"/>
       <c r="F19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="38" t="s">
-        <v>95</v>
-      </c>
+      <c r="G19" s="38"/>
       <c r="H19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="38" t="s">
-        <v>88</v>
-      </c>
+      <c r="I19" s="38"/>
       <c r="J19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="39" t="s">
-        <v>88</v>
-      </c>
+      <c r="K19" s="39"/>
       <c r="L19" s="11"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="83" t="s">
+      <c r="C20" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="111" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="112"/>
-      <c r="F20" s="111" t="s">
+      <c r="D20" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="115"/>
+      <c r="F20" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="112"/>
-      <c r="H20" s="111" t="s">
+      <c r="G20" s="115"/>
+      <c r="H20" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="112"/>
-      <c r="J20" s="111" t="s">
+      <c r="I20" s="115"/>
+      <c r="J20" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="113"/>
+      <c r="K20" s="116"/>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="82"/>
-      <c r="C21" s="91"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="123"/>
       <c r="D21" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="E21" s="26"/>
       <c r="F21" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="G21" s="26"/>
       <c r="H21" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="I21" s="26"/>
       <c r="J21" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="K21" s="27"/>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="81"/>
-      <c r="C22" s="86"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="124"/>
       <c r="D22" s="43"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="38" t="s">
-        <v>88</v>
-      </c>
+      <c r="G22" s="38"/>
       <c r="H22" s="46"/>
       <c r="I22" s="44"/>
       <c r="J22" s="46"/>
@@ -2310,59 +2270,51 @@
       <c r="B23" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="115" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="116"/>
-      <c r="F23" s="115" t="s">
+      <c r="D23" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="92"/>
+      <c r="F23" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="116"/>
-      <c r="H23" s="115" t="s">
+      <c r="G23" s="92"/>
+      <c r="H23" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="116"/>
-      <c r="J23" s="105" t="s">
+      <c r="I23" s="92"/>
+      <c r="J23" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="114"/>
+      <c r="K23" s="118"/>
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="74"/>
-      <c r="C24" s="97"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="E24" s="26"/>
       <c r="F24" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="G24" s="26"/>
       <c r="H24" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I24" s="26"/>
       <c r="J24" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="K24" s="27"/>
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="74"/>
-      <c r="C25" s="88"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="34"/>
       <c r="E25" s="29"/>
       <c r="F25" s="34"/>
@@ -2372,49 +2324,43 @@
       <c r="J25" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="K25" s="49" t="s">
-        <v>88</v>
-      </c>
+      <c r="K25" s="49"/>
       <c r="L25" s="8"/>
     </row>
     <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="74"/>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="95" t="s">
+      <c r="D26" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="96"/>
-      <c r="F26" s="95" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="96"/>
-      <c r="H26" s="95" t="s">
+      <c r="E26" s="89"/>
+      <c r="F26" s="88" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="89"/>
+      <c r="H26" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="96"/>
-      <c r="J26" s="98" t="s">
+      <c r="I26" s="89"/>
+      <c r="J26" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="145"/>
+      <c r="K26" s="82"/>
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="74"/>
-      <c r="C27" s="97"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="E27" s="26"/>
       <c r="F27" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="G27" s="26"/>
       <c r="H27" s="25" t="s">
         <v>7</v>
       </c>
@@ -2427,7 +2373,7 @@
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="74"/>
-      <c r="C28" s="88"/>
+      <c r="C28" s="113"/>
       <c r="D28" s="34"/>
       <c r="E28" s="29"/>
       <c r="F28" s="34"/>
@@ -2442,67 +2388,57 @@
     </row>
     <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="74"/>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="144"/>
-      <c r="F29" s="120" t="s">
+      <c r="E29" s="81"/>
+      <c r="F29" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="120"/>
-      <c r="H29" s="98" t="s">
+      <c r="G29" s="90"/>
+      <c r="H29" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="I29" s="144"/>
-      <c r="J29" s="98" t="s">
+      <c r="I29" s="81"/>
+      <c r="J29" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="145"/>
+      <c r="K29" s="82"/>
       <c r="L29" s="8"/>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="74"/>
-      <c r="C30" s="97"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="E30" s="26"/>
       <c r="F30" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="G30" s="26"/>
       <c r="H30" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I30" s="26"/>
       <c r="J30" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="K30" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="K30" s="27"/>
       <c r="L30" s="8"/>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="74"/>
-      <c r="C31" s="97"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="E31" s="26"/>
       <c r="F31" s="51"/>
       <c r="G31" s="29"/>
       <c r="H31" s="52"/>
@@ -2514,13 +2450,11 @@
     </row>
     <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="74"/>
-      <c r="C32" s="97"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="E32" s="26"/>
       <c r="F32" s="51"/>
       <c r="G32" s="29"/>
       <c r="H32" s="52"/>
@@ -2532,13 +2466,11 @@
     </row>
     <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="74"/>
-      <c r="C33" s="97"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="54" t="s">
-        <v>88</v>
-      </c>
+      <c r="E33" s="54"/>
       <c r="F33" s="51"/>
       <c r="G33" s="29"/>
       <c r="H33" s="55"/>
@@ -2550,57 +2482,49 @@
     </row>
     <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="74"/>
-      <c r="C34" s="97"/>
-      <c r="D34" s="98" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" s="99"/>
-      <c r="F34" s="98" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" s="144"/>
-      <c r="H34" s="120" t="s">
+      <c r="C34" s="86"/>
+      <c r="D34" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="145"/>
+      <c r="F34" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="81"/>
+      <c r="H34" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="120"/>
-      <c r="J34" s="98" t="s">
+      <c r="I34" s="90"/>
+      <c r="J34" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="K34" s="121"/>
+      <c r="K34" s="100"/>
       <c r="L34" s="8"/>
     </row>
     <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="74"/>
-      <c r="C35" s="97"/>
+      <c r="C35" s="86"/>
       <c r="D35" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="E35" s="26"/>
       <c r="F35" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="G35" s="26"/>
       <c r="H35" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I35" s="26"/>
       <c r="J35" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K35" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="K35" s="27"/>
       <c r="L35" s="8"/>
     </row>
     <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="75"/>
-      <c r="C36" s="77"/>
+      <c r="C36" s="87"/>
       <c r="D36" s="58"/>
       <c r="E36" s="59"/>
       <c r="F36" s="58"/>
@@ -2608,124 +2532,106 @@
       <c r="H36" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="38" t="s">
-        <v>88</v>
-      </c>
+      <c r="I36" s="38"/>
       <c r="J36" s="58"/>
       <c r="K36" s="62"/>
       <c r="L36" s="8"/>
     </row>
     <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C37" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="122" t="s">
+      <c r="D37" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="127"/>
-      <c r="F37" s="122" t="s">
+      <c r="E37" s="84"/>
+      <c r="F37" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="127"/>
-      <c r="H37" s="122" t="s">
+      <c r="G37" s="84"/>
+      <c r="H37" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="I37" s="127"/>
-      <c r="J37" s="122" t="s">
+      <c r="I37" s="84"/>
+      <c r="J37" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="K37" s="123"/>
+      <c r="K37" s="101"/>
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="82"/>
-      <c r="C38" s="84"/>
+      <c r="B38" s="137"/>
+      <c r="C38" s="138"/>
       <c r="D38" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="54" t="s">
-        <v>88</v>
-      </c>
+      <c r="E38" s="54"/>
       <c r="F38" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="54" t="s">
-        <v>95</v>
-      </c>
+      <c r="G38" s="54"/>
       <c r="H38" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I38" s="54" t="s">
-        <v>88</v>
-      </c>
+      <c r="I38" s="54"/>
       <c r="J38" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="K38" s="39" t="s">
-        <v>88</v>
-      </c>
+      <c r="K38" s="39"/>
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="82"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="137"/>
+      <c r="C39" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D39" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="125"/>
-      <c r="F39" s="124" t="s">
+      <c r="E39" s="103"/>
+      <c r="F39" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="125"/>
-      <c r="H39" s="131" t="s">
-        <v>101</v>
-      </c>
-      <c r="I39" s="132"/>
-      <c r="J39" s="126" t="s">
+      <c r="G39" s="103"/>
+      <c r="H39" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="109"/>
+      <c r="J39" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="K39" s="128"/>
+      <c r="K39" s="105"/>
       <c r="L39" s="1"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="82"/>
-      <c r="C40" s="91"/>
+      <c r="B40" s="137"/>
+      <c r="C40" s="123"/>
       <c r="D40" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="E40" s="26"/>
       <c r="F40" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="G40" s="26"/>
       <c r="H40" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="I40" s="26" t="s">
-        <v>88</v>
-      </c>
+      <c r="I40" s="26"/>
       <c r="J40" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="K40" s="27"/>
       <c r="L40" s="1"/>
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="82"/>
-      <c r="C41" s="84"/>
+      <c r="B41" s="137"/>
+      <c r="C41" s="138"/>
       <c r="D41" s="66"/>
       <c r="E41" s="67"/>
       <c r="F41" s="66"/>
@@ -2733,40 +2639,38 @@
       <c r="H41" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="54" t="s">
-        <v>88</v>
-      </c>
+      <c r="I41" s="54"/>
       <c r="J41" s="66"/>
       <c r="K41" s="68"/>
       <c r="L41" s="1"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="82"/>
-      <c r="C42" s="85" t="s">
+      <c r="B42" s="137"/>
+      <c r="C42" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="124" t="s">
+      <c r="D42" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="125"/>
-      <c r="F42" s="124" t="s">
+      <c r="E42" s="103"/>
+      <c r="F42" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="G42" s="125"/>
-      <c r="H42" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42" s="130"/>
-      <c r="J42" s="124" t="s">
+      <c r="G42" s="103"/>
+      <c r="H42" s="107" t="s">
+        <v>100</v>
+      </c>
+      <c r="I42" s="107"/>
+      <c r="J42" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="K42" s="129"/>
+      <c r="K42" s="106"/>
       <c r="L42" s="8"/>
     </row>
     <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="81"/>
-      <c r="C43" s="86"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="124"/>
       <c r="D43" s="69" t="s">
         <v>7</v>
       </c>
@@ -2789,30 +2693,30 @@
       <c r="B44" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="87" t="s">
+      <c r="C44" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="115" t="s">
+      <c r="D44" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="116"/>
-      <c r="F44" s="115" t="s">
+      <c r="E44" s="92"/>
+      <c r="F44" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="G44" s="116"/>
-      <c r="H44" s="115" t="s">
-        <v>106</v>
-      </c>
-      <c r="I44" s="116"/>
-      <c r="J44" s="115" t="s">
+      <c r="G44" s="92"/>
+      <c r="H44" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="I44" s="92"/>
+      <c r="J44" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="K44" s="135"/>
+      <c r="K44" s="96"/>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="74"/>
-      <c r="C45" s="88"/>
+      <c r="C45" s="113"/>
       <c r="D45" s="48" t="s">
         <v>7</v>
       </c>
@@ -2833,30 +2737,30 @@
     </row>
     <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="74"/>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="95" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="139"/>
-      <c r="F46" s="133" t="s">
+      <c r="D46" s="88" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="93"/>
+      <c r="F46" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="134"/>
-      <c r="H46" s="139" t="s">
-        <v>107</v>
-      </c>
-      <c r="I46" s="139"/>
-      <c r="J46" s="133" t="s">
+      <c r="G46" s="95"/>
+      <c r="H46" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="93"/>
+      <c r="J46" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="K46" s="136"/>
+      <c r="K46" s="97"/>
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="74"/>
-      <c r="C47" s="93"/>
+      <c r="C47" s="143"/>
       <c r="D47" s="25" t="s">
         <v>7</v>
       </c>
@@ -2877,7 +2781,7 @@
     </row>
     <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="75"/>
-      <c r="C48" s="94"/>
+      <c r="C48" s="144"/>
       <c r="D48" s="58"/>
       <c r="E48" s="59"/>
       <c r="F48" s="71" t="s">
@@ -2891,33 +2795,33 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="80" t="s">
+      <c r="B49" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="89" t="s">
+      <c r="C49" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="122" t="s">
+      <c r="D49" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="127"/>
-      <c r="F49" s="122" t="s">
+      <c r="E49" s="84"/>
+      <c r="F49" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="G49" s="127"/>
-      <c r="H49" s="122" t="s">
+      <c r="G49" s="84"/>
+      <c r="H49" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="I49" s="127"/>
-      <c r="J49" s="137" t="s">
+      <c r="I49" s="84"/>
+      <c r="J49" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="K49" s="138"/>
+      <c r="K49" s="99"/>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="81"/>
-      <c r="C50" s="90"/>
+      <c r="B50" s="136"/>
+      <c r="C50" s="141"/>
       <c r="D50" s="43" t="s">
         <v>7</v>
       </c>
@@ -2937,8 +2841,68 @@
       <c r="L50" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qHxMlw49t7cqo6EtZn1JiBEwhCFMVlVf09HtocEiB3234myTQ3Iz4EJJRZvPPi8M/sZ/XjG+4AZMQVCjHtmYJw==" saltValue="ptowAI5jvPGgMLBWmqqr8w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jcaQVtr6ICyvfZG8CdnzDqla+wpPzBO0P7BBCI+k8jRiH7jHIwAm8gbmyPf2HBUjrwZN5KNmZBSOC+RmCJRx0w==" saltValue="2AN9Xe05nMKjoDp+BeQfGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="76">
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H44:I44"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="C13:C17"/>
     <mergeCell ref="D29:E29"/>
@@ -2955,66 +2919,6 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K27:K28 G14 E14 E19 G19 I19 K19 I16 G21:G22 K14:K16 E21 I21 K21 I24 G24 E24 E27 G27 G30 E35 I35:I36 G40 E40 K35 K40 E47 I47 E30:E33 G35 I38 K38 G38 E38 I40:I41 K43 I43 G43 E43 E45 E50 G50 G47:G48 I50 K50 K45 I45 G45 I30 K30 I27 K24:K25 I14 K47" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">
@@ -3039,9 +2943,7 @@
   </sheetPr>
   <dimension ref="B2:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3085,24 +2987,24 @@
         <v>68</v>
       </c>
       <c r="D3" s="13">
-        <f>IF('Diagnostic Questions'!E14="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!E14="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f>IF('Diagnostic Questions'!G14="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!G14="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="F3" s="13">
-        <f>0.5*IF('Diagnostic Questions'!I14="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I16="Yes",1,0)</f>
-        <v>1</v>
+        <f>0.5*IF('DRM Diagnostic'!I14="Yes",1,0) + 0.5*IF('DRM Diagnostic'!I16="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="G3" s="13">
-        <f>ROUND(0.3333*IF('Diagnostic Questions'!K14="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K15="Yes",1,0) + 0.3333*IF('Diagnostic Questions'!K16="Yes",1,0),2)</f>
+        <f>ROUND(0.3333*IF('DRM Diagnostic'!K14="Yes",1,0) + 0.3333*IF('DRM Diagnostic'!K15="Yes",1,0) + 0.3333*IF('DRM Diagnostic'!K16="Yes",1,0),2)</f>
         <v>0</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B3:G3)</f>
-        <v>Legal and Institutional DRM Framework,DRM policies and institutions,1,1,1,0</v>
+        <v>Legal and Institutional DRM Framework,DRM policies and institutions,0,0,0,0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -3113,24 +3015,24 @@
         <v>69</v>
       </c>
       <c r="D4" s="13">
-        <f>IF('Diagnostic Questions'!E19="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E19="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E4" s="13">
-        <f>IF('Diagnostic Questions'!G19="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G19="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <f>IF('Diagnostic Questions'!I19="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!I19="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="G4" s="13">
-        <f>IF('Diagnostic Questions'!K19="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!K19="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,B4:G4)</f>
-        <v>Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,1,1</v>
+        <v>Legal and Institutional DRM Framework,Mainstreaming DRM into national and sectoral development plans,0,0,0,0</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -3138,27 +3040,27 @@
         <v>70</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="13">
-        <f>IF('Diagnostic Questions'!E21="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E21="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E5" s="13">
-        <f>0.5*IF('Diagnostic Questions'!G21="Yes",1,0) + 0.5*IF('Diagnostic Questions'!G22="Yes",1,0)</f>
-        <v>0.5</v>
+        <f>0.5*IF('DRM Diagnostic'!G21="Yes",1,0) + 0.5*IF('DRM Diagnostic'!G22="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="F5" s="13">
-        <f>IF('Diagnostic Questions'!I21="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I21="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G5" s="13">
-        <f>IF('Diagnostic Questions'!K21="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!K21="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I14" si="0">_xlfn.TEXTJOIN(",",FALSE,B5:G5)</f>
-        <v>Risk Identification,Risk identification,0,0.5,0,1</v>
+        <v>Risk Identification,Risk identification,0,0,0,0</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -3169,24 +3071,24 @@
         <v>71</v>
       </c>
       <c r="D6" s="13">
-        <f>IF('Diagnostic Questions'!E24="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!E24="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="E6" s="13">
-        <f>IF('Diagnostic Questions'!G24="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!G24="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="F6" s="13">
-        <f>IF('Diagnostic Questions'!I24="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!I24="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="G6" s="13">
-        <f>0.5*IF('Diagnostic Questions'!K24="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K25="Yes",1,0)</f>
-        <v>1</v>
+        <f>0.5*IF('DRM Diagnostic'!K24="Yes",1,0) + 0.5*IF('DRM Diagnostic'!K25="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>Risk Reduction,Territorial and urban planning,1,1,1,1</v>
+        <v>Risk Reduction,Territorial and urban planning,0,0,0,0</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -3197,19 +3099,19 @@
         <v>72</v>
       </c>
       <c r="D7" s="13">
-        <f>IF('Diagnostic Questions'!E27="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E27="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E7" s="13">
-        <f>IF('Diagnostic Questions'!G27="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G27="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F7" s="13">
-        <f>IF('Diagnostic Questions'!I27="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I27="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G7" s="13">
-        <f>0.5*IF('Diagnostic Questions'!K27="Yes",1,0) + 0.5*IF('Diagnostic Questions'!K28="Yes",1,0)</f>
+        <f>0.5*IF('DRM Diagnostic'!K27="Yes",1,0) + 0.5*IF('DRM Diagnostic'!K28="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="I7" t="str">
@@ -3225,24 +3127,24 @@
         <v>73</v>
       </c>
       <c r="D8" s="13">
-        <f>0.2*IF('Diagnostic Questions'!E30="Yes",1,0)+0.2*IF('Diagnostic Questions'!E31="Yes",1,0)+0.2*IF('Diagnostic Questions'!E32="Yes",1,0)+0.2*IF('Diagnostic Questions'!E33="Yes",1,0)+0.2*IF('Diagnostic Questions'!E35="Yes",1,0)</f>
-        <v>0.8</v>
+        <f>0.2*IF('DRM Diagnostic'!E30="Yes",1,0)+0.2*IF('DRM Diagnostic'!E31="Yes",1,0)+0.2*IF('DRM Diagnostic'!E32="Yes",1,0)+0.2*IF('DRM Diagnostic'!E33="Yes",1,0)+0.2*IF('DRM Diagnostic'!E35="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="E8" s="13">
-        <f>0.5*IF('Diagnostic Questions'!G30="Yes",1,0)+0.5*IF('Diagnostic Questions'!G35="Yes",1,0)</f>
-        <v>0.5</v>
+        <f>0.5*IF('DRM Diagnostic'!G30="Yes",1,0)+0.5*IF('DRM Diagnostic'!G35="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="F8" s="13">
-        <f>ROUND(0.3333*IF('Diagnostic Questions'!I30="Yes",1,0)+0.3333*IF('Diagnostic Questions'!I35="Yes",1,0)+0.3333*IF('Diagnostic Questions'!I36="Yes",1,0),2)</f>
-        <v>1</v>
+        <f>ROUND(0.3333*IF('DRM Diagnostic'!I30="Yes",1,0)+0.3333*IF('DRM Diagnostic'!I35="Yes",1,0)+0.3333*IF('DRM Diagnostic'!I36="Yes",1,0),2)</f>
+        <v>0</v>
       </c>
       <c r="G8" s="13">
-        <f>0.5*IF('Diagnostic Questions'!K30="Yes",1,0)+0.5*IF('Diagnostic Questions'!K35="Yes",1,0)</f>
-        <v>1</v>
+        <f>0.5*IF('DRM Diagnostic'!K30="Yes",1,0)+0.5*IF('DRM Diagnostic'!K35="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>Risk Reduction,Sector-specific risk reduction measures,0.8,0.5,1,1</v>
+        <v>Risk Reduction,Sector-specific risk reduction measures,0,0,0,0</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -3250,27 +3152,27 @@
         <v>78</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="13">
-        <f>IF('Diagnostic Questions'!E38="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!E38="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="E9" s="13">
-        <f>IF('Diagnostic Questions'!G38="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G38="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F9" s="13">
-        <f>IF('Diagnostic Questions'!I38="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!I38="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="G9" s="13">
-        <f>IF('Diagnostic Questions'!K38="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!K38="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>Preparedness,Early warning systems,1,0,1,1</v>
+        <v>Preparedness,Early warning systems,0,0,0,0</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -3278,27 +3180,27 @@
         <v>78</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="13">
-        <f>IF('Diagnostic Questions'!E40="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E40="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E10" s="13">
-        <f>IF('Diagnostic Questions'!G40="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G40="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F10" s="13">
-        <f>0.5*IF('Diagnostic Questions'!I40="Yes",1,0) + 0.5*IF('Diagnostic Questions'!I41="Yes",1,0)</f>
-        <v>1</v>
+        <f>0.5*IF('DRM Diagnostic'!I40="Yes",1,0) + 0.5*IF('DRM Diagnostic'!I41="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="G10" s="13">
-        <f>IF('Diagnostic Questions'!K40="Yes",1,0)</f>
-        <v>1</v>
+        <f>IF('DRM Diagnostic'!K40="Yes",1,0)</f>
+        <v>0</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>Preparedness,Emergency preparedness and response,0,0,1,1</v>
+        <v>Preparedness,Emergency preparedness and response,0,0,0,0</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -3306,22 +3208,22 @@
         <v>78</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="13">
-        <f>IF('Diagnostic Questions'!E43="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E43="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E11" s="13">
-        <f>IF('Diagnostic Questions'!G43="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G43="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F11" s="13">
-        <f>IF('Diagnostic Questions'!I43="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I43="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G11" s="13">
-        <f>IF('Diagnostic Questions'!K43="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!K43="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="I11" t="str">
@@ -3337,19 +3239,19 @@
         <v>74</v>
       </c>
       <c r="D12" s="13">
-        <f>IF('Diagnostic Questions'!E45="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E45="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E12" s="13">
-        <f>IF('Diagnostic Questions'!G45="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G45="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F12" s="13">
-        <f>IF('Diagnostic Questions'!I45="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I45="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G12" s="13">
-        <f>IF('Diagnostic Questions'!K45="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!K45="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="I12" t="str">
@@ -3362,22 +3264,22 @@
         <v>79</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="13">
-        <f>IF('Diagnostic Questions'!E47="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E47="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="13">
-        <f>0.5*IF('Diagnostic Questions'!G47="Yes",1,0)+0.5*IF('Diagnostic Questions'!G48="Yes",1,0)</f>
+        <f>0.5*IF('DRM Diagnostic'!G47="Yes",1,0)+0.5*IF('DRM Diagnostic'!G48="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F13" s="13">
-        <f>IF('Diagnostic Questions'!I47="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I47="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G13" s="13">
-        <f>IF('Diagnostic Questions'!K47="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!K47="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="I13" t="str">
@@ -3390,22 +3292,22 @@
         <v>75</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="13">
-        <f>IF('Diagnostic Questions'!E50="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!E50="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="E14" s="13">
-        <f>IF('Diagnostic Questions'!G50="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!G50="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="13">
-        <f>IF('Diagnostic Questions'!I50="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!I50="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="G14" s="13">
-        <f>IF('Diagnostic Questions'!K50="Yes",1,0)</f>
+        <f>IF('DRM Diagnostic'!K50="Yes",1,0)</f>
         <v>0</v>
       </c>
       <c r="I14" t="str">
@@ -3418,13 +3320,14 @@
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="20"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="guScLaW1msqZa/7T/I6g5INETt6eOkQCzQBLfjTVWBj9GnsPd5IIrA1ePwMv55yqQPYajoQnKigGfNGxKzW7yg==" saltValue="FpjmMvsD1dnzZDAeHqznCA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update guidelines and references in app layout
Revised the guidelines section in app.py for clarity and updated references from cell D7 to E7 to match the latest Excel template. Removed redundant explanations and adjusted instructions to align with the new structure of the diagnostic tool. Updated the Excel template to reflect these changes.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B997EEB-7916-4D71-823D-9183477A5203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9B997EEB-7916-4D71-823D-9183477A5203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC29F9FD-F7BC-4805-84B0-793E980A1272}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -418,6 +418,18 @@
   </si>
   <si>
     <t>Are there legal and institutional arrangements for water supply and sanitation in urban areas that take flood risk into account?</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Question 4</t>
   </si>
 </sst>
 </file>
@@ -1311,19 +1323,87 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1331,259 +1411,191 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1937,7 +1949,9 @@
   </sheetPr>
   <dimension ref="B2:AU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1974,15 +1988,15 @@
       </c>
     </row>
     <row r="6" spans="2:47" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="134" t="s">
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="134"/>
+      <c r="F6" s="79"/>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
@@ -2015,22 +2029,22 @@
       <c r="C12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="129"/>
-      <c r="F12" s="127" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="129"/>
-      <c r="H12" s="127" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="129"/>
-      <c r="J12" s="127" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="128"/>
+      <c r="D12" s="102" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="104"/>
+      <c r="F12" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="104"/>
+      <c r="H12" s="102" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="104"/>
+      <c r="J12" s="102" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" s="103"/>
       <c r="L12" s="9"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -2072,30 +2086,30 @@
       <c r="B13" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="117" t="s">
+      <c r="D13" s="105" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="117" t="s">
+      <c r="E13" s="106"/>
+      <c r="F13" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="130"/>
-      <c r="H13" s="131" t="s">
+      <c r="G13" s="106"/>
+      <c r="H13" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="I13" s="132"/>
-      <c r="J13" s="125" t="s">
+      <c r="I13" s="108"/>
+      <c r="J13" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="K13" s="126"/>
+      <c r="K13" s="101"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="74"/>
-      <c r="C14" s="77"/>
+      <c r="C14" s="141"/>
       <c r="D14" s="23" t="s">
         <v>7</v>
       </c>
@@ -2116,7 +2130,7 @@
     </row>
     <row r="15" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="74"/>
-      <c r="C15" s="78"/>
+      <c r="C15" s="142"/>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="F15" s="28"/>
@@ -2131,7 +2145,7 @@
     </row>
     <row r="16" spans="2:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="74"/>
-      <c r="C16" s="78"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
       <c r="F16" s="28"/>
@@ -2148,7 +2162,7 @@
     </row>
     <row r="17" spans="2:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="74"/>
-      <c r="C17" s="79"/>
+      <c r="C17" s="143"/>
       <c r="D17" s="34"/>
       <c r="E17" s="29"/>
       <c r="F17" s="34"/>
@@ -2161,31 +2175,31 @@
     </row>
     <row r="18" spans="2:14" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74"/>
-      <c r="C18" s="85" t="s">
+      <c r="C18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="110" t="s">
+      <c r="D18" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="119"/>
-      <c r="F18" s="120" t="s">
+      <c r="E18" s="117"/>
+      <c r="F18" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="119"/>
-      <c r="H18" s="120" t="s">
+      <c r="G18" s="117"/>
+      <c r="H18" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="121"/>
-      <c r="J18" s="110" t="s">
+      <c r="I18" s="119"/>
+      <c r="J18" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="111"/>
+      <c r="K18" s="110"/>
       <c r="L18" s="10"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="75"/>
-      <c r="C19" s="87"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="37" t="s">
         <v>7</v>
       </c>
@@ -2206,33 +2220,33 @@
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="2:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="114" t="s">
+      <c r="D20" s="111" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="115"/>
-      <c r="F20" s="114" t="s">
+      <c r="E20" s="112"/>
+      <c r="F20" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="115"/>
-      <c r="H20" s="114" t="s">
+      <c r="G20" s="112"/>
+      <c r="H20" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="115"/>
-      <c r="J20" s="114" t="s">
+      <c r="I20" s="112"/>
+      <c r="J20" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="116"/>
+      <c r="K20" s="113"/>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="137"/>
-      <c r="C21" s="123"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="40" t="s">
         <v>7</v>
       </c>
@@ -2252,8 +2266,8 @@
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="136"/>
-      <c r="C22" s="124"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="43"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45" t="s">
@@ -2270,30 +2284,30 @@
       <c r="B23" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="112" t="s">
+      <c r="C23" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="D23" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="92"/>
-      <c r="F23" s="91" t="s">
+      <c r="E23" s="116"/>
+      <c r="F23" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="92"/>
-      <c r="H23" s="91" t="s">
+      <c r="G23" s="116"/>
+      <c r="H23" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="92"/>
-      <c r="J23" s="117" t="s">
+      <c r="I23" s="116"/>
+      <c r="J23" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="118"/>
+      <c r="K23" s="114"/>
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="74"/>
-      <c r="C24" s="86"/>
+      <c r="C24" s="97"/>
       <c r="D24" s="25" t="s">
         <v>7</v>
       </c>
@@ -2314,7 +2328,7 @@
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="74"/>
-      <c r="C25" s="113"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="34"/>
       <c r="E25" s="29"/>
       <c r="F25" s="34"/>
@@ -2329,30 +2343,30 @@
     </row>
     <row r="26" spans="2:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="74"/>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="88" t="s">
+      <c r="D26" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="89"/>
-      <c r="F26" s="88" t="s">
+      <c r="E26" s="96"/>
+      <c r="F26" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="G26" s="89"/>
-      <c r="H26" s="88" t="s">
+      <c r="G26" s="96"/>
+      <c r="H26" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="89"/>
-      <c r="J26" s="80" t="s">
+      <c r="I26" s="96"/>
+      <c r="J26" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="82"/>
+      <c r="K26" s="145"/>
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="74"/>
-      <c r="C27" s="86"/>
+      <c r="C27" s="97"/>
       <c r="D27" s="25" t="s">
         <v>7</v>
       </c>
@@ -2373,7 +2387,7 @@
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="74"/>
-      <c r="C28" s="113"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="34"/>
       <c r="E28" s="29"/>
       <c r="F28" s="34"/>
@@ -2388,31 +2402,31 @@
     </row>
     <row r="29" spans="2:14" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="74"/>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="80" t="s">
+      <c r="D29" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="81"/>
-      <c r="F29" s="90" t="s">
+      <c r="E29" s="144"/>
+      <c r="F29" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="90"/>
-      <c r="H29" s="80" t="s">
+      <c r="G29" s="120"/>
+      <c r="H29" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I29" s="81"/>
-      <c r="J29" s="80" t="s">
+      <c r="I29" s="144"/>
+      <c r="J29" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="82"/>
+      <c r="K29" s="145"/>
       <c r="L29" s="8"/>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="74"/>
-      <c r="C30" s="86"/>
+      <c r="C30" s="97"/>
       <c r="D30" s="31" t="s">
         <v>60</v>
       </c>
@@ -2434,7 +2448,7 @@
     </row>
     <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="74"/>
-      <c r="C31" s="86"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="31" t="s">
         <v>61</v>
       </c>
@@ -2450,7 +2464,7 @@
     </row>
     <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="74"/>
-      <c r="C32" s="86"/>
+      <c r="C32" s="97"/>
       <c r="D32" s="31" t="s">
         <v>63</v>
       </c>
@@ -2466,7 +2480,7 @@
     </row>
     <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="74"/>
-      <c r="C33" s="86"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="48" t="s">
         <v>64</v>
       </c>
@@ -2482,28 +2496,28 @@
     </row>
     <row r="34" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="74"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="80" t="s">
+      <c r="C34" s="97"/>
+      <c r="D34" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="145"/>
-      <c r="F34" s="80" t="s">
+      <c r="E34" s="99"/>
+      <c r="F34" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G34" s="81"/>
-      <c r="H34" s="90" t="s">
+      <c r="G34" s="144"/>
+      <c r="H34" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="90"/>
-      <c r="J34" s="80" t="s">
+      <c r="I34" s="120"/>
+      <c r="J34" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="K34" s="100"/>
+      <c r="K34" s="121"/>
       <c r="L34" s="8"/>
     </row>
     <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="74"/>
-      <c r="C35" s="86"/>
+      <c r="C35" s="97"/>
       <c r="D35" s="25" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2538,7 @@
     </row>
     <row r="36" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="75"/>
-      <c r="C36" s="87"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="58"/>
       <c r="E36" s="59"/>
       <c r="F36" s="58"/>
@@ -2538,33 +2552,33 @@
       <c r="L36" s="8"/>
     </row>
     <row r="37" spans="2:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="135" t="s">
+      <c r="B37" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="122" t="s">
+      <c r="C37" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="83" t="s">
+      <c r="D37" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="84"/>
-      <c r="F37" s="83" t="s">
+      <c r="E37" s="127"/>
+      <c r="F37" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="84"/>
-      <c r="H37" s="83" t="s">
+      <c r="G37" s="127"/>
+      <c r="H37" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="I37" s="84"/>
-      <c r="J37" s="83" t="s">
+      <c r="I37" s="127"/>
+      <c r="J37" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="K37" s="101"/>
+      <c r="K37" s="123"/>
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="137"/>
-      <c r="C38" s="138"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="63" t="s">
         <v>7</v>
       </c>
@@ -2584,32 +2598,32 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="137"/>
-      <c r="C39" s="139" t="s">
+      <c r="B39" s="82"/>
+      <c r="C39" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="104" t="s">
+      <c r="D39" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="103"/>
-      <c r="F39" s="102" t="s">
+      <c r="E39" s="125"/>
+      <c r="F39" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="103"/>
-      <c r="H39" s="108" t="s">
+      <c r="G39" s="125"/>
+      <c r="H39" s="131" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="109"/>
-      <c r="J39" s="104" t="s">
+      <c r="I39" s="132"/>
+      <c r="J39" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="K39" s="105"/>
+      <c r="K39" s="128"/>
       <c r="L39" s="1"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="137"/>
-      <c r="C40" s="123"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="91"/>
       <c r="D40" s="64" t="s">
         <v>7</v>
       </c>
@@ -2630,8 +2644,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="137"/>
-      <c r="C41" s="138"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="84"/>
       <c r="D41" s="66"/>
       <c r="E41" s="67"/>
       <c r="F41" s="66"/>
@@ -2646,31 +2660,31 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="2:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="137"/>
-      <c r="C42" s="139" t="s">
+      <c r="B42" s="82"/>
+      <c r="C42" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="102" t="s">
+      <c r="D42" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="103"/>
-      <c r="F42" s="102" t="s">
+      <c r="E42" s="125"/>
+      <c r="F42" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="G42" s="103"/>
-      <c r="H42" s="107" t="s">
+      <c r="G42" s="125"/>
+      <c r="H42" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="I42" s="107"/>
-      <c r="J42" s="102" t="s">
+      <c r="I42" s="130"/>
+      <c r="J42" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="K42" s="106"/>
+      <c r="K42" s="129"/>
       <c r="L42" s="8"/>
     </row>
     <row r="43" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="136"/>
-      <c r="C43" s="124"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="86"/>
       <c r="D43" s="69" t="s">
         <v>7</v>
       </c>
@@ -2693,30 +2707,30 @@
       <c r="B44" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="112" t="s">
+      <c r="C44" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="91" t="s">
+      <c r="D44" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="92"/>
-      <c r="F44" s="91" t="s">
+      <c r="E44" s="116"/>
+      <c r="F44" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="G44" s="92"/>
-      <c r="H44" s="91" t="s">
+      <c r="G44" s="116"/>
+      <c r="H44" s="115" t="s">
         <v>104</v>
       </c>
-      <c r="I44" s="92"/>
-      <c r="J44" s="91" t="s">
+      <c r="I44" s="116"/>
+      <c r="J44" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="K44" s="96"/>
+      <c r="K44" s="135"/>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="74"/>
-      <c r="C45" s="113"/>
+      <c r="C45" s="88"/>
       <c r="D45" s="48" t="s">
         <v>7</v>
       </c>
@@ -2737,30 +2751,30 @@
     </row>
     <row r="46" spans="2:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="74"/>
-      <c r="C46" s="142" t="s">
+      <c r="C46" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="88" t="s">
+      <c r="D46" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="93"/>
-      <c r="F46" s="94" t="s">
+      <c r="E46" s="139"/>
+      <c r="F46" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="95"/>
-      <c r="H46" s="93" t="s">
+      <c r="G46" s="134"/>
+      <c r="H46" s="139" t="s">
         <v>105</v>
       </c>
-      <c r="I46" s="93"/>
-      <c r="J46" s="94" t="s">
+      <c r="I46" s="139"/>
+      <c r="J46" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="K46" s="97"/>
+      <c r="K46" s="136"/>
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="74"/>
-      <c r="C47" s="143"/>
+      <c r="C47" s="93"/>
       <c r="D47" s="25" t="s">
         <v>7</v>
       </c>
@@ -2781,7 +2795,7 @@
     </row>
     <row r="48" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="75"/>
-      <c r="C48" s="144"/>
+      <c r="C48" s="94"/>
       <c r="D48" s="58"/>
       <c r="E48" s="59"/>
       <c r="F48" s="71" t="s">
@@ -2795,33 +2809,33 @@
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="2:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="135" t="s">
+      <c r="B49" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="140" t="s">
+      <c r="C49" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="83" t="s">
+      <c r="D49" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="84"/>
-      <c r="F49" s="83" t="s">
+      <c r="E49" s="127"/>
+      <c r="F49" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="G49" s="84"/>
-      <c r="H49" s="83" t="s">
+      <c r="G49" s="127"/>
+      <c r="H49" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="I49" s="84"/>
-      <c r="J49" s="98" t="s">
+      <c r="I49" s="127"/>
+      <c r="J49" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="K49" s="99"/>
+      <c r="K49" s="138"/>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="136"/>
-      <c r="C50" s="141"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="90"/>
       <c r="D50" s="43" t="s">
         <v>7</v>
       </c>
@@ -2843,6 +2857,66 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="jcaQVtr6ICyvfZG8CdnzDqla+wpPzBO0P7BBCI+k8jRiH7jHIwAm8gbmyPf2HBUjrwZN5KNmZBSOC+RmCJRx0w==" saltValue="2AN9Xe05nMKjoDp+BeQfGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="76">
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B23:B36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="B6:D6"/>
@@ -2859,66 +2933,6 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B23:B36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F34:G34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K27:K28 G14 E14 E19 G19 I19 K19 I16 G21:G22 K14:K16 E21 I21 K21 I24 G24 E24 E27 G27 G30 E35 I35:I36 G40 E40 K35 K40 E47 I47 E30:E33 G35 I38 K38 G38 E38 I40:I41 K43 I43 G43 E43 E45 E50 G50 G47:G48 I50 K50 K45 I45 G45 I30 K30 I27 K24:K25 I14 K47" xr:uid="{4F850B23-72D3-42CE-AFF7-E77C4B7FF2EF}">

</xml_diff>

<commit_message>
Refactor data parsing and chart generation logic
Moved question mapping and parsing logic to config and utils modules, enabling direct parsing of pasted Q#,Yes/No,Weight data. Replaced figure_generator.py with petal_chart_figure_generator.py and added pillar_chart.py for modular chart creation. Updated app.py to use new parsing and chart functions, simplified results workflow, and refreshed UI text and styles for clarity. Removed legacy table code and unused CSS.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874EDB9-B754-46F2-8BC8-E7A612AC2DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E8F8F-D387-46E5-8CF0-859394472AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="DRM Diagnostic" sheetId="5" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of questions unanswered: </t>
-  </si>
-  <si>
     <t>Thematic Area</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
   </si>
   <si>
     <t>Do laws and regulations mandate the use of risk information (e.g., hazard maps, risk assessments) to develop territorial, spatial, land use, or urban planning instruments?</t>
-  </si>
-  <si>
-    <t>DRM Diagnostic</t>
   </si>
   <si>
     <t>Is there a legal framework (e.g., a DRM law or other legally-binding instruments) defining distinct responsibilities for disaster risk reduction and emergency management?</t>
@@ -442,12 +436,18 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Blanks</t>
+  </si>
+  <si>
+    <t>Disaster Risk Management Policy Diagnostic Tool</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,13 +538,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -940,7 +933,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1094,37 +1087,40 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1143,13 +1139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1497,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605CE87-02FF-4583-93E8-6522C5287CD6}">
-  <dimension ref="B2:AY201"/>
+  <dimension ref="B2:AY198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1516,13 +1506,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:51" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1535,24 +1525,27 @@
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
+      <c r="G7" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="54"/>
@@ -1560,7 +1553,10 @@
       <c r="D8" s="49"/>
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
+      <c r="G8" s="4">
+        <f>COUNTBLANK(E15:E61)</f>
+        <v>0</v>
+      </c>
       <c r="H8" s="50"/>
       <c r="I8" s="51"/>
       <c r="J8" s="51"/>
@@ -1608,7 +1604,7 @@
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="52"/>
       <c r="D9" s="49"/>
@@ -1661,15 +1657,15 @@
       <c r="AY9" s="51"/>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B10" s="58" t="str">
-        <f>IF(B13&gt;0,"Please complete asessment to proceed", _xlfn.TEXTJOIN(";",FALSE,H18:H64))</f>
-        <v>Q1,Yes,1;Q2,No,1;Q3,No,0.5;Q4,Yes,0.5;Q5,No,1;Q6,Yes,1;Q7,No,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,No,1;Q12,No,0.5;Q13,Yes,0.5;Q14,Yes,1;Q15,No,1;Q16,Yes,1;Q17,Yes,1;Q18,No,0.25;Q19,No,0.25;Q20,Yes,0.25;Q21,Yes,0.25;Q22,No,1;Q23,Yes,1;Q24,No,1;Q25,No,1;Q26,No,0.5;Q27,No,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,No,0.5;Q33,No,0.5;Q34,Yes,1;Q35,Yes,1;Q36,Yes,1;Q37,Yes,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,Yes,1;Q43,Yes,1;Q44,Yes,1;Q45,Yes,1;Q46,No,1;Q47,Yes,1</v>
-      </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="50"/>
+      <c r="B10" s="57" t="str">
+        <f>IF(G8&gt;0,_xlfn.CONCAT("Please complete asessment to proceed. Remaining questions: ",G8), _xlfn.TEXTJOIN(";",FALSE,H15:H61))</f>
+        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,No,1;Q6,Yes,1;Q7,No,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,No,1;Q12,No,0.5;Q13,Yes,0.5;Q14,Yes,1;Q15,No,1;Q16,Yes,1;Q17,Yes,1;Q18,No,0.25;Q19,No,0.25;Q20,Yes,0.25;Q21,Yes,0.25;Q22,No,1;Q23,Yes,1;Q24,No,1;Q25,No,1;Q26,No,0.5;Q27,No,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,No,0.5;Q33,No,0.5;Q34,Yes,1;Q35,Yes,1;Q36,Yes,1;Q37,Yes,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,Yes,1;Q43,Yes,1;Q44,Yes,1;Q45,Yes,1;Q46,No,1;Q47,Yes,1</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="50" t="s">
+        <v>124</v>
+      </c>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="50"/>
@@ -1721,1019 +1717,1008 @@
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="2:51" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B13" s="55">
-        <f>47-(COUNTIF(E17:E64,"YES")+COUNTIF(E17:E64,"NO"))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B15" s="56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="2:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="D14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
+      <c r="G15" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,G15,E15,F15)</f>
+        <v>Q1,Yes,1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="58"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="37">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f t="shared" ref="H16:H61" si="0">_xlfn.TEXTJOIN(",",FALSE,G16,E16,F16)</f>
+        <v>Q2,Yes,1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q3,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="58"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q4,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="58"/>
+      <c r="C19" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="36">
+        <v>1</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q5,No,1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="58"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="38">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q6,Yes,1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="69"/>
+      <c r="D21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="39">
+        <v>1</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q7,No,1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="58"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q8,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="58"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q9,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="73"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="40">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q10,Yes,1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="41">
+        <v>1</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q11,No,1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="58"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q12,No,0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="58"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q13,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="58"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="37">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q14,Yes,1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="58"/>
+      <c r="C29" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="36">
+        <v>1</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q15,No,1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="58"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="22" t="s">
+      <c r="E30" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="37">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q16,Yes,1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="58"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="36">
+        <v>1</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q17,Yes,1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="58"/>
+      <c r="C32" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q18,No,0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="58"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="25" t="s">
+      <c r="E33" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="36">
-        <v>1</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(",",FALSE,G18,E18,F18)</f>
-        <v>Q1,Yes,1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="72"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="37">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" ref="H19:H64" si="0">_xlfn.TEXTJOIN(",",FALSE,G19,E19,F19)</f>
-        <v>Q2,No,1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="72"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="36">
+      <c r="F33" s="36">
+        <v>0.25</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q19,No,0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="58"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q20,Yes,0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="58"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="36">
+        <v>0.25</v>
+      </c>
+      <c r="G35" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q21,Yes,0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="58"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="37">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q22,No,1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="58"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="36">
+        <v>1</v>
+      </c>
+      <c r="G37" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q23,Yes,1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="58"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="37">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q24,No,1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="58"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="36">
+        <v>1</v>
+      </c>
+      <c r="G39" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="H39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q25,No,1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="58"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="37">
         <v>0.5</v>
       </c>
-      <c r="G20" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q3,No,0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="72"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="6" t="s">
+      <c r="G40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q26,No,0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="58"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="H41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q27,No,0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="43">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q28,Yes,1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="60"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="36">
+        <v>1</v>
+      </c>
+      <c r="G43" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q29,Yes,1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="60"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="37">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q30,Yes,1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="60"/>
+      <c r="C45" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="36">
+        <v>1</v>
+      </c>
+      <c r="G45" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q31,Yes,1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="60"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E46" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F46" s="37">
         <v>0.5</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q4,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="72"/>
-      <c r="C22" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="36">
-        <v>1</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q5,No,1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="72"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="G46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q32,No,0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="60"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="38">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q6,Yes,1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="39">
-        <v>1</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q7,No,1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="72"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="26" t="s">
+      <c r="F47" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="G47" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q33,No,0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="60"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="37">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q34,Yes,1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="60"/>
+      <c r="C49" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="36">
+        <v>1</v>
+      </c>
+      <c r="G49" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="H49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q35,Yes,1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="60"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="37">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q36,Yes,1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="61"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="44">
+        <v>1</v>
+      </c>
+      <c r="G51" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="H51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q37,Yes,1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="45">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q38,Yes,1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="60"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="36">
+        <v>1</v>
+      </c>
+      <c r="G53" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="H53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q39,Yes,1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="60"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q40,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="60"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="H55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q41,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="60"/>
+      <c r="C56" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="37">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q42,Yes,1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="60"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="36">
+        <v>1</v>
+      </c>
+      <c r="G57" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q43,Yes,1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="60"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="38">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q44,Yes,1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="69"/>
+      <c r="D59" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="39">
+        <v>1</v>
+      </c>
+      <c r="G59" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="H59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q45,Yes,1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="60"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q8,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="72"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q9,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="73"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="40">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q10,Yes,1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="41">
-        <v>1</v>
-      </c>
-      <c r="G28" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="H28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q11,No,1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="72"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q12,No,0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="72"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q13,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="72"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="37">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q14,Yes,1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="72"/>
-      <c r="C32" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="36">
-        <v>1</v>
-      </c>
-      <c r="G32" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="H32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q15,No,1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="72"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="37">
-        <v>1</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q16,Yes,1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="36">
-        <v>1</v>
-      </c>
-      <c r="G34" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="H34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q17,Yes,1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="72"/>
-      <c r="C35" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="37">
-        <v>0.25</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q18,No,0.25</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="72"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="36">
-        <v>0.25</v>
-      </c>
-      <c r="G36" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q19,No,0.25</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="72"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="37">
-        <v>0.25</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q20,Yes,0.25</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="72"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="36">
-        <v>0.25</v>
-      </c>
-      <c r="G38" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q21,Yes,0.25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="72"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="37">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q22,No,1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="72"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="36">
-        <v>1</v>
-      </c>
-      <c r="G40" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q23,Yes,1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="72"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="37">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q24,No,1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="72"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="36">
-        <v>1</v>
-      </c>
-      <c r="G42" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="H42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q25,No,1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="72"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q26,No,0.5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="72"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F44" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="G44" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q27,No,0.5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="43">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q28,Yes,1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="61"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F46" s="36">
-        <v>1</v>
-      </c>
-      <c r="G46" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="H46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q29,Yes,1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="61"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" s="37">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q30,Yes,1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="61"/>
-      <c r="C48" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="36">
-        <v>1</v>
-      </c>
-      <c r="G48" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q31,Yes,1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="61"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F49" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q32,No,0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="61"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="G50" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q33,No,0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="61"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" s="37">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q34,Yes,1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="61"/>
-      <c r="C52" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F52" s="36">
-        <v>1</v>
-      </c>
-      <c r="G52" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="H52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q35,Yes,1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="61"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" s="37">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q36,Yes,1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="62"/>
-      <c r="C54" s="67"/>
-      <c r="D54" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E54" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" s="44">
-        <v>1</v>
-      </c>
-      <c r="G54" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q37,Yes,1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E55" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" s="45">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q38,Yes,1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="61"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" s="36">
-        <v>1</v>
-      </c>
-      <c r="G56" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="H56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q39,Yes,1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="61"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q40,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="61"/>
-      <c r="C58" s="64"/>
-      <c r="D58" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="G58" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="H58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q41,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="61"/>
-      <c r="C59" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" s="37">
-        <v>1</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q42,Yes,1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="61"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" s="36">
-        <v>1</v>
-      </c>
-      <c r="G60" s="47" t="s">
-        <v>119</v>
+      <c r="F60" s="37">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q43,Yes,1</v>
+        <v>Q46,No,1</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="61"/>
-      <c r="C61" s="63"/>
-      <c r="D61" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E61" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" s="38">
-        <v>1</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>120</v>
+      <c r="C61" s="71"/>
+      <c r="D61" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" s="44">
+        <v>1</v>
+      </c>
+      <c r="G61" s="47" t="s">
+        <v>121</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q44,Yes,1</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C62" s="68"/>
-      <c r="D62" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E62" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" s="39">
-        <v>1</v>
-      </c>
-      <c r="G62" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="H62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q45,Yes,1</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="61"/>
-      <c r="C63" s="69"/>
-      <c r="D63" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E63" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" s="37">
-        <v>1</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q46,No,1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="62"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="F64" s="44">
-        <v>1</v>
-      </c>
-      <c r="G64" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="H64" s="1" t="str">
-        <f t="shared" si="0"/>
         <v>Q47,Yes,1</v>
       </c>
     </row>
+    <row r="62" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2868,34 +2853,31 @@
     <row r="196" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="197" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="198" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B18:B23"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C56:C58"/>
     <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B28:B44"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="B25:B41"/>
+    <mergeCell ref="B42:B51"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B20"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18:E64" xr:uid="{DDBFF9BC-A376-44E4-9EF0-101A8F72CB94}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:E61" xr:uid="{DDBFF9BC-A376-44E4-9EF0-101A8F72CB94}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Refactor thematic area display and improve pillar chart color mapping
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E8F8F-D387-46E5-8CF0-859394472AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B141C54-6498-4028-A82E-FE297890BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Question</t>
@@ -1094,52 +1091,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1489,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605CE87-02FF-4583-93E8-6522C5287CD6}">
   <dimension ref="B2:AY198"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1506,13 +1503,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="B2" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:51" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1525,26 +1522,26 @@
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
       <c r="G7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1604,7 +1601,7 @@
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="52"/>
       <c r="D9" s="49"/>
@@ -1659,12 +1656,12 @@
     <row r="10" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="str">
         <f>IF(G8&gt;0,_xlfn.CONCAT("Please complete asessment to proceed. Remaining questions: ",G8), _xlfn.TEXTJOIN(";",FALSE,H15:H61))</f>
-        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,No,1;Q6,Yes,1;Q7,No,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,No,1;Q12,No,0.5;Q13,Yes,0.5;Q14,Yes,1;Q15,No,1;Q16,Yes,1;Q17,Yes,1;Q18,No,0.25;Q19,No,0.25;Q20,Yes,0.25;Q21,Yes,0.25;Q22,No,1;Q23,Yes,1;Q24,No,1;Q25,No,1;Q26,No,0.5;Q27,No,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,No,0.5;Q33,No,0.5;Q34,Yes,1;Q35,Yes,1;Q36,Yes,1;Q37,Yes,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,Yes,1;Q43,Yes,1;Q44,Yes,1;Q45,Yes,1;Q46,No,1;Q47,Yes,1</v>
+        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,Yes,1;Q6,Yes,1;Q7,Yes,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,Yes,1;Q12,Yes,0.5;Q13,Yes,0.5;Q14,Yes,1;Q15,Yes,1;Q16,Yes,1;Q17,Yes,1;Q18,Yes,0.25;Q19,Yes,0.25;Q20,Yes,0.25;Q21,Yes,0.25;Q22,Yes,1;Q23,Yes,1;Q24,Yes,1;Q25,Yes,1;Q26,Yes,0.5;Q27,Yes,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,Yes,0.5;Q33,Yes,0.5;Q34,Yes,1;Q35,Yes,1;Q36,Yes,1;Q37,Yes,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,Yes,1;Q43,Yes,1;Q44,Yes,1;Q45,Yes,1;Q46,Yes,1;Q47,Yes,1</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="53"/>
       <c r="E10" s="50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
@@ -1718,7 +1715,7 @@
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B12" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1732,36 +1729,36 @@
         <v>32</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="36">
-        <v>1</v>
-      </c>
-      <c r="G15" s="47" t="s">
-        <v>75</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,G15,E15,F15)</f>
@@ -1769,8 +1766,8 @@
       </c>
     </row>
     <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
-      <c r="C16" s="63"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1781,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" ref="H16:H61" si="0">_xlfn.TEXTJOIN(",",FALSE,G16,E16,F16)</f>
@@ -1789,10 +1786,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
-      <c r="C17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>45</v>
@@ -1801,7 +1798,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1809,10 +1806,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="26" t="s">
         <v>45</v>
@@ -1821,82 +1818,82 @@
         <v>0.5</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q4,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="71"/>
+      <c r="C19" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="36">
+        <v>1</v>
+      </c>
+      <c r="G19" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q4,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
-      <c r="C19" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q5,Yes,1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="71"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="36">
-        <v>1</v>
-      </c>
-      <c r="G19" s="47" t="s">
+      <c r="E20" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="38">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q5,No,1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="58"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="38">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Q6,Yes,1</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="39">
         <v>1</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q7,No,1</v>
+        <v>Q7,Yes,1</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="58"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>45</v>
@@ -1905,7 +1902,7 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1913,10 +1910,10 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="58"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>45</v>
@@ -1925,7 +1922,7 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1933,8 +1930,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="73"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
@@ -1945,60 +1942,60 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q10,Yes,1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="41">
+        <v>1</v>
+      </c>
+      <c r="G25" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q10,Yes,1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="41">
-        <v>1</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>85</v>
-      </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q11,No,1</v>
+        <v>Q11,Yes,1</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="58"/>
-      <c r="C26" s="63"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="37">
         <v>0.5</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q12,No,0.5</v>
+        <v>Q12,Yes,0.5</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="C27" s="63"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="10" t="s">
         <v>38</v>
       </c>
@@ -2009,58 +2006,58 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q13,Yes,0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="71"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="37">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q13,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="58"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="37">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Q14,Yes,1</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="58"/>
-      <c r="C29" s="62" t="s">
+      <c r="B29" s="71"/>
+      <c r="C29" s="64" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="36">
         <v>1</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q15,No,1</v>
+        <v>Q15,Yes,1</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="58"/>
-      <c r="C30" s="63"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="6" t="s">
         <v>33</v>
       </c>
@@ -2071,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2079,8 +2076,8 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="58"/>
-      <c r="C31" s="64"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="10" t="s">
         <v>41</v>
       </c>
@@ -2091,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2099,52 +2096,52 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="58"/>
-      <c r="C32" s="62" t="s">
+      <c r="B32" s="71"/>
+      <c r="C32" s="64" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" s="37">
         <v>0.25</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q18,No,0.25</v>
+        <v>Q18,Yes,0.25</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="58"/>
-      <c r="C33" s="63"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="36">
         <v>0.25</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q19,No,0.25</v>
+        <v>Q19,Yes,0.25</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="58"/>
-      <c r="C34" s="63"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>45</v>
@@ -2153,7 +2150,7 @@
         <v>0.25</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2161,10 +2158,10 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="58"/>
-      <c r="C35" s="63"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>45</v>
@@ -2173,7 +2170,7 @@
         <v>0.25</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2181,28 +2178,28 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="58"/>
-      <c r="C36" s="63"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" s="37">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q22,No,1</v>
+        <v>Q22,Yes,1</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="58"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="10" t="s">
         <v>40</v>
       </c>
@@ -2213,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2221,90 +2218,90 @@
       </c>
     </row>
     <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="58"/>
-      <c r="C38" s="63"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F38" s="37">
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q24,Yes,1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="71"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="36">
+        <v>1</v>
+      </c>
+      <c r="G39" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q24,No,1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="58"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="36">
-        <v>1</v>
-      </c>
-      <c r="G39" s="47" t="s">
-        <v>99</v>
-      </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q25,No,1</v>
+        <v>Q25,Yes,1</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="58"/>
-      <c r="C40" s="63"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F40" s="37">
         <v>0.5</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q26,No,0.5</v>
+        <v>Q26,Yes,0.5</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="58"/>
-      <c r="C41" s="63"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F41" s="42">
         <v>0.5</v>
       </c>
       <c r="G41" s="47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q27,No,0.5</v>
+        <v>Q27,Yes,0.5</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -2317,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2326,7 +2323,7 @@
     </row>
     <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="60"/>
-      <c r="C43" s="63"/>
+      <c r="C43" s="62"/>
       <c r="D43" s="10" t="s">
         <v>15</v>
       </c>
@@ -2337,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2346,7 +2343,7 @@
     </row>
     <row r="44" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="60"/>
-      <c r="C44" s="64"/>
+      <c r="C44" s="63"/>
       <c r="D44" s="6" t="s">
         <v>16</v>
       </c>
@@ -2357,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2366,7 +2363,7 @@
     </row>
     <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="60"/>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="64" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -2379,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2388,47 +2385,47 @@
     </row>
     <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="60"/>
-      <c r="C46" s="63"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F46" s="37">
         <v>0.5</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q32,No,0.5</v>
+        <v>Q32,Yes,0.5</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="60"/>
-      <c r="C47" s="63"/>
+      <c r="C47" s="62"/>
       <c r="D47" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F47" s="36">
         <v>0.5</v>
       </c>
       <c r="G47" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q33,No,0.5</v>
+        <v>Q33,Yes,0.5</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="60"/>
-      <c r="C48" s="64"/>
+      <c r="C48" s="63"/>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
@@ -2439,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2448,7 +2445,7 @@
     </row>
     <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="60"/>
-      <c r="C49" s="62" t="s">
+      <c r="C49" s="64" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="10" t="s">
@@ -2461,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2470,7 +2467,7 @@
     </row>
     <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="60"/>
-      <c r="C50" s="63"/>
+      <c r="C50" s="62"/>
       <c r="D50" s="6" t="s">
         <v>22</v>
       </c>
@@ -2481,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2490,9 +2487,9 @@
     </row>
     <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="61"/>
-      <c r="C51" s="68"/>
+      <c r="C51" s="66"/>
       <c r="D51" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E51" s="33" t="s">
         <v>45</v>
@@ -2501,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2512,7 +2509,7 @@
       <c r="B52" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="63" t="s">
+      <c r="C52" s="62" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="8" t="s">
@@ -2525,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2534,7 +2531,7 @@
     </row>
     <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="60"/>
-      <c r="C53" s="63"/>
+      <c r="C53" s="62"/>
       <c r="D53" s="10" t="s">
         <v>25</v>
       </c>
@@ -2545,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2554,7 +2551,7 @@
     </row>
     <row r="54" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="60"/>
-      <c r="C54" s="63"/>
+      <c r="C54" s="62"/>
       <c r="D54" s="6" t="s">
         <v>34</v>
       </c>
@@ -2565,7 +2562,7 @@
         <v>0.5</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2574,7 +2571,7 @@
     </row>
     <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="60"/>
-      <c r="C55" s="64"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="10" t="s">
         <v>26</v>
       </c>
@@ -2585,7 +2582,7 @@
         <v>0.5</v>
       </c>
       <c r="G55" s="47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2594,7 +2591,7 @@
     </row>
     <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="60"/>
-      <c r="C56" s="62" t="s">
+      <c r="C56" s="64" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -2607,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2616,7 +2613,7 @@
     </row>
     <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="60"/>
-      <c r="C57" s="63"/>
+      <c r="C57" s="62"/>
       <c r="D57" s="10" t="s">
         <v>44</v>
       </c>
@@ -2627,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2636,9 +2633,9 @@
     </row>
     <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B58" s="60"/>
-      <c r="C58" s="63"/>
+      <c r="C58" s="62"/>
       <c r="D58" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E58" s="27" t="s">
         <v>45</v>
@@ -2647,7 +2644,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2658,7 +2655,7 @@
       <c r="B59" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="69"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="11" t="s">
         <v>29</v>
       </c>
@@ -2669,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2678,27 +2675,27 @@
     </row>
     <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="60"/>
-      <c r="C60" s="70"/>
+      <c r="C60" s="68"/>
       <c r="D60" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F60" s="37">
         <v>1</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q46,No,1</v>
+        <v>Q46,Yes,1</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="61"/>
-      <c r="C61" s="71"/>
+      <c r="C61" s="69"/>
       <c r="D61" s="16" t="s">
         <v>30</v>
       </c>
@@ -2709,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2855,6 +2852,9 @@
     <row r="198" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B20"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="C25:C28"/>
@@ -2871,9 +2871,6 @@
     <mergeCell ref="B25:B41"/>
     <mergeCell ref="B42:B51"/>
     <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B20"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Add LLM-based summaries and country selection UI
Introduces helper functions to generate answer indicators and load LLM-generated summaries for thematic areas from JSON files. Adds a country selection dropdown to the input form and updates the app layout to support new summary and country features.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B141C54-6498-4028-A82E-FE297890BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="126">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -930,7 +930,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1117,15 +1117,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1486,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605CE87-02FF-4583-93E8-6522C5287CD6}">
   <dimension ref="B2:AY198"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,8 +1488,8 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="87.21875" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="6.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="6.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1742,7 +1733,7 @@
       </c>
     </row>
     <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="70" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="64" t="s">
@@ -1766,7 +1757,7 @@
       </c>
     </row>
     <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="62"/>
       <c r="D16" s="6" t="s">
         <v>3</v>
@@ -1786,7 +1777,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="62"/>
       <c r="D17" s="10" t="s">
         <v>56</v>
@@ -1806,7 +1797,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="71"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="63"/>
       <c r="D18" s="6" t="s">
         <v>57</v>
@@ -1826,7 +1817,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="64" t="s">
         <v>4</v>
       </c>
@@ -1848,7 +1839,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="71"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="62"/>
       <c r="D20" s="7" t="s">
         <v>66</v>
@@ -1868,10 +1859,12 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="67"/>
+      <c r="C21" s="67" t="s">
+        <v>5</v>
+      </c>
       <c r="D21" s="11" t="s">
         <v>35</v>
       </c>
@@ -1890,7 +1883,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="71"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="68"/>
       <c r="D22" s="6" t="s">
         <v>61</v>
@@ -1910,7 +1903,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="68"/>
       <c r="D23" s="10" t="s">
         <v>62</v>
@@ -1930,7 +1923,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="72"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="69"/>
       <c r="D24" s="12" t="s">
         <v>37</v>
@@ -1950,7 +1943,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="68" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="62" t="s">
@@ -1974,7 +1967,7 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="71"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="62"/>
       <c r="D26" s="6" t="s">
         <v>39</v>
@@ -1994,7 +1987,7 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="71"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="62"/>
       <c r="D27" s="10" t="s">
         <v>38</v>
@@ -2014,7 +2007,7 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="71"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="63"/>
       <c r="D28" s="6" t="s">
         <v>67</v>
@@ -2034,7 +2027,7 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="71"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="64" t="s">
         <v>8</v>
       </c>
@@ -2056,7 +2049,7 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="71"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="62"/>
       <c r="D30" s="6" t="s">
         <v>33</v>
@@ -2076,7 +2069,7 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="71"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="63"/>
       <c r="D31" s="10" t="s">
         <v>41</v>
@@ -2096,7 +2089,7 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="71"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="64" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2111,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="71"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="62"/>
       <c r="D33" s="20" t="s">
         <v>51</v>
@@ -2138,7 +2131,7 @@
       </c>
     </row>
     <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="71"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="62"/>
       <c r="D34" s="21" t="s">
         <v>52</v>
@@ -2158,7 +2151,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="71"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="62"/>
       <c r="D35" s="20" t="s">
         <v>53</v>
@@ -2178,7 +2171,7 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="71"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="62"/>
       <c r="D36" s="6" t="s">
         <v>11</v>
@@ -2198,7 +2191,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="71"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="62"/>
       <c r="D37" s="10" t="s">
         <v>40</v>
@@ -2218,7 +2211,7 @@
       </c>
     </row>
     <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="71"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="62"/>
       <c r="D38" s="6" t="s">
         <v>36</v>
@@ -2238,7 +2231,7 @@
       </c>
     </row>
     <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="71"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="62"/>
       <c r="D39" s="10" t="s">
         <v>70</v>
@@ -2258,7 +2251,7 @@
       </c>
     </row>
     <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="71"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="62"/>
       <c r="D40" s="6" t="s">
         <v>68</v>
@@ -2278,7 +2271,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="71"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="62"/>
       <c r="D41" s="14" t="s">
         <v>69</v>
@@ -2655,7 +2648,9 @@
       <c r="B59" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="67"/>
+      <c r="C59" s="59" t="s">
+        <v>28</v>
+      </c>
       <c r="D59" s="11" t="s">
         <v>29</v>
       </c>
@@ -2675,7 +2670,7 @@
     </row>
     <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="60"/>
-      <c r="C60" s="68"/>
+      <c r="C60" s="60"/>
       <c r="D60" s="6" t="s">
         <v>72</v>
       </c>
@@ -2695,7 +2690,7 @@
     </row>
     <row r="61" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="61"/>
-      <c r="C61" s="69"/>
+      <c r="C61" s="61"/>
       <c r="D61" s="16" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
reduce quality for speed
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jqnmu\OneDrive\World_Bank_DRM\Cat_DDO_DRM_Diagnostic_Dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069234E9-5199-436A-BF0E-0A1396DDCC8E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Disaster Risk Management Policy Diagnostic Tool</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1080,9 +1083,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1091,6 +1091,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1103,15 +1118,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1121,13 +1127,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1477,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605CE87-02FF-4583-93E8-6522C5287CD6}">
   <dimension ref="B2:AY198"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:C61"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,18 +1492,18 @@
     <col min="4" max="4" width="87.21875" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
     <col min="6" max="7" width="6.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:51" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:51" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1526,7 +1529,7 @@
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="4"/>
@@ -1536,7 +1539,7 @@
       </c>
     </row>
     <row r="8" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="54"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="48"/>
       <c r="D8" s="49"/>
       <c r="E8" s="50"/>
@@ -1645,12 +1648,12 @@
       <c r="AY9" s="51"/>
     </row>
     <row r="10" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B10" s="57" t="str">
+      <c r="B10" s="56" t="str">
         <f>IF(G8&gt;0,_xlfn.CONCAT("Please complete asessment to proceed. Remaining questions: ",G8), _xlfn.TEXTJOIN(";",FALSE,H15:H61))</f>
-        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,Yes,1;Q6,Yes,1;Q7,Yes,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,Yes,1;Q12,Yes,0.5;Q13,Yes,0.5;Q14,Yes,1;Q15,Yes,1;Q16,Yes,1;Q17,Yes,1;Q18,Yes,0.25;Q19,Yes,0.25;Q20,Yes,0.25;Q21,Yes,0.25;Q22,Yes,1;Q23,Yes,1;Q24,Yes,1;Q25,Yes,1;Q26,Yes,0.5;Q27,Yes,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,Yes,0.5;Q33,Yes,0.5;Q34,Yes,1;Q35,Yes,1;Q36,Yes,1;Q37,Yes,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,Yes,1;Q43,Yes,1;Q44,Yes,1;Q45,Yes,1;Q46,Yes,1;Q47,Yes,1</v>
-      </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="53"/>
+        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,No,1;Q6,No,1;Q7,Yes,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,No,1;Q12,No,0.5;Q13,No,0.5;Q14,No,1;Q15,Yes,1;Q16,Yes,1;Q17,Yes,1;Q18,No,0.25;Q19,No,0.25;Q20,No,0.25;Q21,No,0.25;Q22,No,1;Q23,No,1;Q24,No,1;Q25,No,1;Q26,No,0.5;Q27,No,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,Yes,0.5;Q33,Yes,0.5;Q34,Yes,1;Q35,No,1;Q36,No,1;Q37,No,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,No,1;Q43,No,1;Q44,No,1;Q45,Yes,1;Q46,Yes,1;Q47,Yes,1</v>
+      </c>
+      <c r="C10" s="55"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="50" t="s">
         <v>123</v>
       </c>
@@ -1705,7 +1708,7 @@
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="54" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1733,10 +1736,10 @@
       </c>
     </row>
     <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="64" t="s">
+      <c r="B15" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="57" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1757,8 +1760,8 @@
       </c>
     </row>
     <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="68"/>
-      <c r="C16" s="62"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1777,8 +1780,8 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="68"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="10" t="s">
         <v>56</v>
       </c>
@@ -1797,8 +1800,8 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="68"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="6" t="s">
         <v>57</v>
       </c>
@@ -1817,15 +1820,15 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="68"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="57" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F19" s="36">
         <v>1</v>
@@ -1835,17 +1838,17 @@
       </c>
       <c r="H19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q5,Yes,1</v>
+        <v>Q5,No,1</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="68"/>
-      <c r="C20" s="62"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F20" s="38">
         <v>1</v>
@@ -1855,14 +1858,14 @@
       </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q6,Yes,1</v>
+        <v>Q6,No,1</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="68" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1883,8 +1886,8 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6" t="s">
         <v>61</v>
       </c>
@@ -1903,8 +1906,8 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="10" t="s">
         <v>62</v>
       </c>
@@ -1943,17 +1946,17 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="58" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>63</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F25" s="41">
         <v>1</v>
@@ -1963,17 +1966,17 @@
       </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q11,Yes,1</v>
+        <v>Q11,No,1</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="68"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F26" s="37">
         <v>0.5</v>
@@ -1983,17 +1986,17 @@
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q12,Yes,0.5</v>
+        <v>Q12,No,0.5</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="68"/>
-      <c r="C27" s="62"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F27" s="36">
         <v>0.5</v>
@@ -2003,17 +2006,17 @@
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q13,Yes,0.5</v>
+        <v>Q13,No,0.5</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="68"/>
-      <c r="C28" s="63"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F28" s="37">
         <v>1</v>
@@ -2023,12 +2026,12 @@
       </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q14,Yes,1</v>
+        <v>Q14,No,1</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="68"/>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="61"/>
+      <c r="C29" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
@@ -2049,8 +2052,8 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="68"/>
-      <c r="C30" s="62"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="58"/>
       <c r="D30" s="6" t="s">
         <v>33</v>
       </c>
@@ -2069,8 +2072,8 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="68"/>
-      <c r="C31" s="63"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="59"/>
       <c r="D31" s="10" t="s">
         <v>41</v>
       </c>
@@ -2089,15 +2092,15 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="68"/>
-      <c r="C32" s="64" t="s">
+      <c r="B32" s="61"/>
+      <c r="C32" s="57" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F32" s="37">
         <v>0.25</v>
@@ -2107,17 +2110,17 @@
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q18,Yes,0.25</v>
+        <v>Q18,No,0.25</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="68"/>
-      <c r="C33" s="62"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="20" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F33" s="36">
         <v>0.25</v>
@@ -2127,17 +2130,17 @@
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q19,Yes,0.25</v>
+        <v>Q19,No,0.25</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="68"/>
-      <c r="C34" s="62"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F34" s="37">
         <v>0.25</v>
@@ -2147,17 +2150,17 @@
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q20,Yes,0.25</v>
+        <v>Q20,No,0.25</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="68"/>
-      <c r="C35" s="62"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="20" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F35" s="36">
         <v>0.25</v>
@@ -2167,17 +2170,17 @@
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q21,Yes,0.25</v>
+        <v>Q21,No,0.25</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="68"/>
-      <c r="C36" s="62"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F36" s="37">
         <v>1</v>
@@ -2187,17 +2190,17 @@
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q22,Yes,1</v>
+        <v>Q22,No,1</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="68"/>
-      <c r="C37" s="62"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="10" t="s">
         <v>40</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F37" s="36">
         <v>1</v>
@@ -2207,17 +2210,17 @@
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q23,Yes,1</v>
+        <v>Q23,No,1</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="68"/>
-      <c r="C38" s="62"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F38" s="37">
         <v>1</v>
@@ -2227,17 +2230,17 @@
       </c>
       <c r="H38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q24,Yes,1</v>
+        <v>Q24,No,1</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="68"/>
-      <c r="C39" s="62"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="58"/>
       <c r="D39" s="10" t="s">
         <v>70</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F39" s="36">
         <v>1</v>
@@ -2247,17 +2250,17 @@
       </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q25,Yes,1</v>
+        <v>Q25,No,1</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="68"/>
-      <c r="C40" s="62"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F40" s="37">
         <v>0.5</v>
@@ -2267,17 +2270,17 @@
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q26,Yes,0.5</v>
+        <v>Q26,No,0.5</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="68"/>
-      <c r="C41" s="62"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="14" t="s">
         <v>69</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F41" s="42">
         <v>0.5</v>
@@ -2287,14 +2290,14 @@
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q27,Yes,0.5</v>
+        <v>Q27,No,0.5</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="59" t="s">
+      <c r="B42" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="65" t="s">
+      <c r="C42" s="66" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -2315,8 +2318,8 @@
       </c>
     </row>
     <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="60"/>
-      <c r="C43" s="62"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="10" t="s">
         <v>15</v>
       </c>
@@ -2335,8 +2338,8 @@
       </c>
     </row>
     <row r="44" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="60"/>
-      <c r="C44" s="63"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="6" t="s">
         <v>16</v>
       </c>
@@ -2355,8 +2358,8 @@
       </c>
     </row>
     <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="60"/>
-      <c r="C45" s="64" t="s">
+      <c r="B45" s="64"/>
+      <c r="C45" s="57" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -2377,8 +2380,8 @@
       </c>
     </row>
     <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="60"/>
-      <c r="C46" s="62"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="6" t="s">
         <v>58</v>
       </c>
@@ -2397,8 +2400,8 @@
       </c>
     </row>
     <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="60"/>
-      <c r="C47" s="62"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="58"/>
       <c r="D47" s="10" t="s">
         <v>59</v>
       </c>
@@ -2417,8 +2420,8 @@
       </c>
     </row>
     <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="60"/>
-      <c r="C48" s="63"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="59"/>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
@@ -2437,15 +2440,15 @@
       </c>
     </row>
     <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="60"/>
-      <c r="C49" s="64" t="s">
+      <c r="B49" s="64"/>
+      <c r="C49" s="57" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F49" s="36">
         <v>1</v>
@@ -2455,17 +2458,17 @@
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q35,Yes,1</v>
+        <v>Q35,No,1</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="60"/>
-      <c r="C50" s="62"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F50" s="37">
         <v>1</v>
@@ -2475,17 +2478,17 @@
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q36,Yes,1</v>
+        <v>Q36,No,1</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="61"/>
-      <c r="C51" s="66"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="67"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F51" s="44">
         <v>1</v>
@@ -2495,14 +2498,14 @@
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q37,Yes,1</v>
+        <v>Q37,No,1</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="62" t="s">
+      <c r="C52" s="58" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="8" t="s">
@@ -2523,8 +2526,8 @@
       </c>
     </row>
     <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="60"/>
-      <c r="C53" s="62"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="10" t="s">
         <v>25</v>
       </c>
@@ -2543,8 +2546,8 @@
       </c>
     </row>
     <row r="54" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="60"/>
-      <c r="C54" s="62"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="58"/>
       <c r="D54" s="6" t="s">
         <v>34</v>
       </c>
@@ -2563,8 +2566,8 @@
       </c>
     </row>
     <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="60"/>
-      <c r="C55" s="63"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="59"/>
       <c r="D55" s="10" t="s">
         <v>26</v>
       </c>
@@ -2583,15 +2586,15 @@
       </c>
     </row>
     <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="60"/>
-      <c r="C56" s="64" t="s">
+      <c r="B56" s="64"/>
+      <c r="C56" s="57" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F56" s="37">
         <v>1</v>
@@ -2601,17 +2604,17 @@
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q42,Yes,1</v>
+        <v>Q42,No,1</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="60"/>
-      <c r="C57" s="62"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="58"/>
       <c r="D57" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F57" s="36">
         <v>1</v>
@@ -2621,17 +2624,17 @@
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q43,Yes,1</v>
+        <v>Q43,No,1</v>
       </c>
     </row>
     <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="60"/>
-      <c r="C58" s="62"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F58" s="38">
         <v>1</v>
@@ -2641,14 +2644,14 @@
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q44,Yes,1</v>
+        <v>Q44,No,1</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="59" t="s">
+      <c r="B59" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="63" t="s">
         <v>28</v>
       </c>
       <c r="D59" s="11" t="s">
@@ -2669,8 +2672,8 @@
       </c>
     </row>
     <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="60"/>
-      <c r="C60" s="60"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
       <c r="D60" s="6" t="s">
         <v>72</v>
       </c>
@@ -2689,8 +2692,8 @@
       </c>
     </row>
     <row r="61" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="61"/>
-      <c r="C61" s="61"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="65"/>
       <c r="D61" s="16" t="s">
         <v>30</v>
       </c>
@@ -2847,6 +2850,9 @@
     <row r="198" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B25:B41"/>
+    <mergeCell ref="B42:B51"/>
+    <mergeCell ref="B52:B58"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B15:B20"/>
@@ -2863,9 +2869,6 @@
     <mergeCell ref="C59:C61"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="C21:C24"/>
-    <mergeCell ref="B25:B41"/>
-    <mergeCell ref="B42:B51"/>
-    <mergeCell ref="B52:B58"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update pillar chart x-axis title for clarity
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069234E9-5199-436A-BF0E-0A1396DDCC8E}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD9D106-83A6-4BEA-8763-1533E50D3AE8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="30612" yWindow="4248" windowWidth="23256" windowHeight="12456" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="DRM Diagnostic" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="125">
   <si>
     <t>DRM Pillar</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Are there regulations that define standards for catastrophe insurance coverage of public or private assets?</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Question</t>
@@ -438,9 +435,6 @@
   </si>
   <si>
     <t>Disaster Risk Management Policy Diagnostic Tool</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1091,6 +1085,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1103,21 +1112,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1128,9 +1125,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1159,6 +1153,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1481,7 +1479,7 @@
   <dimension ref="B2:AY198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,19 +1489,19 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="87.21875" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="6.77734375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="6.77734375" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:51" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="B2" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:51" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1516,26 +1514,26 @@
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
       <c r="G7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1546,7 +1544,7 @@
       <c r="F8" s="50"/>
       <c r="G8" s="4">
         <f>COUNTBLANK(E15:E61)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H8" s="50"/>
       <c r="I8" s="51"/>
@@ -1595,7 +1593,7 @@
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="52"/>
       <c r="D9" s="49"/>
@@ -1650,12 +1648,12 @@
     <row r="10" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B10" s="56" t="str">
         <f>IF(G8&gt;0,_xlfn.CONCAT("Please complete asessment to proceed. Remaining questions: ",G8), _xlfn.TEXTJOIN(";",FALSE,H15:H61))</f>
-        <v>Q1,Yes,1;Q2,Yes,1;Q3,Yes,0.5;Q4,Yes,0.5;Q5,No,1;Q6,No,1;Q7,Yes,1;Q8,Yes,0.5;Q9,Yes,0.5;Q10,Yes,1;Q11,No,1;Q12,No,0.5;Q13,No,0.5;Q14,No,1;Q15,Yes,1;Q16,Yes,1;Q17,Yes,1;Q18,No,0.25;Q19,No,0.25;Q20,No,0.25;Q21,No,0.25;Q22,No,1;Q23,No,1;Q24,No,1;Q25,No,1;Q26,No,0.5;Q27,No,0.5;Q28,Yes,1;Q29,Yes,1;Q30,Yes,1;Q31,Yes,1;Q32,Yes,0.5;Q33,Yes,0.5;Q34,Yes,1;Q35,No,1;Q36,No,1;Q37,No,1;Q38,Yes,1;Q39,Yes,1;Q40,Yes,0.5;Q41,Yes,0.5;Q42,No,1;Q43,No,1;Q44,No,1;Q45,Yes,1;Q46,Yes,1;Q47,Yes,1</v>
+        <v>Please complete asessment to proceed. Remaining questions: 47</v>
       </c>
       <c r="C10" s="55"/>
-      <c r="D10" s="70"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
@@ -1709,7 +1707,7 @@
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B12" s="54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="2:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1723,992 +1721,898 @@
         <v>32</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="36">
-        <v>1</v>
-      </c>
-      <c r="G15" s="47" t="s">
-        <v>74</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,G15,E15,F15)</f>
-        <v>Q1,Yes,1</v>
+        <v>Q1,,1</v>
       </c>
     </row>
     <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="61"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="37">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" ref="H16:H61" si="0">_xlfn.TEXTJOIN(",",FALSE,G16,E16,F16)</f>
-        <v>Q2,Yes,1</v>
+        <v>Q2,,1</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="61"/>
-      <c r="C17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>45</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E17" s="25"/>
       <c r="F17" s="36">
         <v>0.5</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q3,Yes,0.5</v>
+        <v>Q3,,0.5</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="61"/>
-      <c r="C18" s="59"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>45</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E18" s="26"/>
       <c r="F18" s="37">
         <v>0.5</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q4,,0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="58"/>
+      <c r="C19" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="36">
+        <v>1</v>
+      </c>
+      <c r="G19" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q4,Yes,0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="61"/>
-      <c r="C19" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q5,,1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="58"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="36">
-        <v>1</v>
-      </c>
-      <c r="G19" s="47" t="s">
+      <c r="E20" s="27"/>
+      <c r="F20" s="38">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q5,No,1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="61"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="38">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q6,No,1</v>
+        <v>Q6,,1</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="69" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>45</v>
-      </c>
+      <c r="E21" s="28"/>
       <c r="F21" s="39">
         <v>1</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q7,Yes,1</v>
+        <v>Q7,,1</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>45</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E22" s="26"/>
       <c r="F22" s="37">
         <v>0.5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q8,Yes,0.5</v>
+        <v>Q8,,0.5</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>45</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E23" s="25"/>
       <c r="F23" s="36">
         <v>0.5</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q9,Yes,0.5</v>
+        <v>Q9,,0.5</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="E24" s="29"/>
       <c r="F24" s="40">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q10,,1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="41">
+        <v>1</v>
+      </c>
+      <c r="G25" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q10,Yes,1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="58" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="41">
-        <v>1</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>84</v>
-      </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q11,No,1</v>
+        <v>Q11,,1</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
-      <c r="C26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="63"/>
       <c r="D26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="E26" s="26"/>
       <c r="F26" s="37">
         <v>0.5</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q12,No,0.5</v>
+        <v>Q12,,0.5</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="61"/>
-      <c r="C27" s="58"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="63"/>
       <c r="D27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="25" t="s">
-        <v>126</v>
-      </c>
+      <c r="E27" s="25"/>
       <c r="F27" s="36">
         <v>0.5</v>
       </c>
       <c r="G27" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q13,,0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="58"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="37">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q13,No,0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="61"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" s="37">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q14,No,1</v>
+        <v>Q14,,1</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="61"/>
-      <c r="C29" s="57" t="s">
+      <c r="B29" s="58"/>
+      <c r="C29" s="62" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E29" s="25"/>
       <c r="F29" s="36">
         <v>1</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q15,Yes,1</v>
+        <v>Q15,,1</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="61"/>
-      <c r="C30" s="58"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="E30" s="26"/>
       <c r="F30" s="37">
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q16,Yes,1</v>
+        <v>Q16,,1</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="61"/>
-      <c r="C31" s="59"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E31" s="25"/>
       <c r="F31" s="36">
         <v>1</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q17,Yes,1</v>
+        <v>Q17,,1</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="61"/>
-      <c r="C32" s="57" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="62" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>126</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E32" s="26"/>
       <c r="F32" s="37">
         <v>0.25</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q18,No,0.25</v>
+        <v>Q18,,0.25</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
-      <c r="C33" s="58"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="63"/>
       <c r="D33" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>126</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E33" s="25"/>
       <c r="F33" s="36">
         <v>0.25</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q19,No,0.25</v>
+        <v>Q19,,0.25</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="61"/>
-      <c r="C34" s="58"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="63"/>
       <c r="D34" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>126</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E34" s="26"/>
       <c r="F34" s="37">
         <v>0.25</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q20,No,0.25</v>
+        <v>Q20,,0.25</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="61"/>
-      <c r="C35" s="58"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="63"/>
       <c r="D35" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>126</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E35" s="25"/>
       <c r="F35" s="36">
         <v>0.25</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q21,No,0.25</v>
+        <v>Q21,,0.25</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="61"/>
-      <c r="C36" s="58"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="63"/>
       <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="E36" s="26"/>
       <c r="F36" s="37">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q22,No,1</v>
+        <v>Q22,,1</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="61"/>
-      <c r="C37" s="58"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="63"/>
       <c r="D37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="25" t="s">
-        <v>126</v>
-      </c>
+      <c r="E37" s="25"/>
       <c r="F37" s="36">
         <v>1</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q23,No,1</v>
+        <v>Q23,,1</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="61"/>
-      <c r="C38" s="58"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="63"/>
       <c r="D38" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="E38" s="26"/>
       <c r="F38" s="37">
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q24,,1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="58"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="36">
+        <v>1</v>
+      </c>
+      <c r="G39" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q24,No,1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="61"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F39" s="36">
-        <v>1</v>
-      </c>
-      <c r="G39" s="47" t="s">
-        <v>98</v>
-      </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q25,No,1</v>
+        <v>Q25,,1</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="61"/>
-      <c r="C40" s="58"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="63"/>
       <c r="D40" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>126</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E40" s="26"/>
       <c r="F40" s="37">
         <v>0.5</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q26,No,0.5</v>
+        <v>Q26,,0.5</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="61"/>
-      <c r="C41" s="58"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>126</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E41" s="31"/>
       <c r="F41" s="42">
         <v>0.5</v>
       </c>
       <c r="G41" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q27,No,0.5</v>
+        <v>Q27,,0.5</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="67" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="E42" s="32"/>
       <c r="F42" s="43">
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q28,Yes,1</v>
+        <v>Q28,,1</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="64"/>
-      <c r="C43" s="58"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="63"/>
       <c r="D43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E43" s="25"/>
       <c r="F43" s="36">
         <v>1</v>
       </c>
       <c r="G43" s="47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q29,Yes,1</v>
+        <v>Q29,,1</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="64"/>
-      <c r="C44" s="59"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="64"/>
       <c r="D44" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="E44" s="26"/>
       <c r="F44" s="37">
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q30,Yes,1</v>
+        <v>Q30,,1</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="64"/>
-      <c r="C45" s="57" t="s">
+      <c r="B45" s="60"/>
+      <c r="C45" s="62" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E45" s="25"/>
       <c r="F45" s="36">
         <v>1</v>
       </c>
       <c r="G45" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q31,Yes,1</v>
+        <v>Q31,,1</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="64"/>
-      <c r="C46" s="58"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="63"/>
       <c r="D46" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>45</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E46" s="26"/>
       <c r="F46" s="37">
         <v>0.5</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q32,Yes,0.5</v>
+        <v>Q32,,0.5</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="64"/>
-      <c r="C47" s="58"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="63"/>
       <c r="D47" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>45</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E47" s="25"/>
       <c r="F47" s="36">
         <v>0.5</v>
       </c>
       <c r="G47" s="47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q33,Yes,0.5</v>
+        <v>Q33,,0.5</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="64"/>
-      <c r="C48" s="59"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="64"/>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="E48" s="26"/>
       <c r="F48" s="37">
         <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q34,Yes,1</v>
+        <v>Q34,,1</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="64"/>
-      <c r="C49" s="57" t="s">
+      <c r="B49" s="60"/>
+      <c r="C49" s="62" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="25" t="s">
-        <v>126</v>
-      </c>
+      <c r="E49" s="25"/>
       <c r="F49" s="36">
         <v>1</v>
       </c>
       <c r="G49" s="47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q35,No,1</v>
+        <v>Q35,,1</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="64"/>
-      <c r="C50" s="58"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="63"/>
       <c r="D50" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="E50" s="26"/>
       <c r="F50" s="37">
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q36,,1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="61"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="33"/>
+      <c r="F51" s="44">
+        <v>1</v>
+      </c>
+      <c r="G51" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="H50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q36,No,1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="65"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="F51" s="44">
-        <v>1</v>
-      </c>
-      <c r="G51" s="47" t="s">
-        <v>110</v>
-      </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q37,No,1</v>
+        <v>Q37,,1</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="64" t="s">
+      <c r="B52" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="63" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="34" t="s">
-        <v>45</v>
-      </c>
+      <c r="E52" s="34"/>
       <c r="F52" s="45">
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q38,Yes,1</v>
+        <v>Q38,,1</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="64"/>
-      <c r="C53" s="58"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="63"/>
       <c r="D53" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E53" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E53" s="25"/>
       <c r="F53" s="36">
         <v>1</v>
       </c>
       <c r="G53" s="47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q39,Yes,1</v>
+        <v>Q39,,1</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="64"/>
-      <c r="C54" s="58"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="63"/>
       <c r="D54" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="E54" s="26"/>
       <c r="F54" s="37">
         <v>0.5</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q40,Yes,0.5</v>
+        <v>Q40,,0.5</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="64"/>
-      <c r="C55" s="59"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="64"/>
       <c r="D55" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="E55" s="25"/>
       <c r="F55" s="36">
         <v>0.5</v>
       </c>
       <c r="G55" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q41,Yes,0.5</v>
+        <v>Q41,,0.5</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="64"/>
-      <c r="C56" s="57" t="s">
+      <c r="B56" s="60"/>
+      <c r="C56" s="62" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E56" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="E56" s="26"/>
       <c r="F56" s="37">
         <v>1</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q42,No,1</v>
+        <v>Q42,,1</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="64"/>
-      <c r="C57" s="58"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="63"/>
       <c r="D57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="25" t="s">
-        <v>126</v>
-      </c>
+      <c r="E57" s="25"/>
       <c r="F57" s="36">
         <v>1</v>
       </c>
       <c r="G57" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q43,,1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="60"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="27"/>
+      <c r="F58" s="38">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q43,No,1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="64"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="F58" s="38">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q44,No,1</v>
+        <v>Q44,,1</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="63" t="s">
+      <c r="B59" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="63" t="s">
+      <c r="C59" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E59" s="35" t="s">
-        <v>45</v>
-      </c>
+      <c r="E59" s="35"/>
       <c r="F59" s="39">
         <v>1</v>
       </c>
       <c r="G59" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q45,,1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="60"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" s="26"/>
+      <c r="F60" s="37">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Q45,Yes,1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F60" s="37">
-        <v>1</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q46,Yes,1</v>
+        <v>Q46,,1</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="65"/>
-      <c r="C61" s="65"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="61"/>
       <c r="D61" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="33" t="s">
-        <v>45</v>
-      </c>
+      <c r="E61" s="33"/>
       <c r="F61" s="44">
         <v>1</v>
       </c>
       <c r="G61" s="47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Q47,Yes,1</v>
+        <v>Q47,,1</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2850,12 +2754,6 @@
     <row r="198" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B25:B41"/>
-    <mergeCell ref="B42:B51"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B20"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="C25:C28"/>
@@ -2869,6 +2767,12 @@
     <mergeCell ref="C59:C61"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="C21:C24"/>
+    <mergeCell ref="B25:B41"/>
+    <mergeCell ref="B42:B51"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B20"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update DRM System Diagnostic Assessment template
Replaces the existing DRM System Diagnostic Assessment - Template.xlsx file with a new version. The update may include revised content, formatting, or data improvements.
</commit_message>
<xml_diff>
--- a/data/DRM System Diagnostic Assessment - Template.xlsx
+++ b/data/DRM System Diagnostic Assessment - Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62bed0b45625b526/World_Bank_DRM/Cat_DDO_DRM_Diagnostic_Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD9D106-83A6-4BEA-8763-1533E50D3AE8}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{E281060C-B249-4EEA-A958-CD0BF3134DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE9760BC-03E1-47FE-84C7-EE3490DF81FB}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="4248" windowWidth="23256" windowHeight="12456" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D35593D8-ABCE-4EA8-921D-2F7793671AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="DRM Diagnostic" sheetId="5" r:id="rId1"/>
@@ -179,12 +179,6 @@
     <t>1. Answer the questions below.</t>
   </si>
   <si>
-    <t>2. Go to the following website. The website may take some time to load, please retry if needed.</t>
-  </si>
-  <si>
-    <t>https://cat-ddo-drm-diagnostic-dashboard.onrender.com</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -435,6 +429,12 @@
   </si>
   <si>
     <t>Disaster Risk Management Policy Diagnostic Tool</t>
+  </si>
+  <si>
+    <t>https://cat-ddo-drm-diagnostic-dashboard-129737065802.us-central1.run.app/</t>
+  </si>
+  <si>
+    <t>2. Go to the following website for the latest version of the tool. The website may take some time to load, please retry if needed.</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1088,45 +1088,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -1479,7 +1480,7 @@
   <dimension ref="B2:AY198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,13 +1496,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="B2" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:51" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1521,19 +1522,19 @@
     </row>
     <row r="6" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="53" t="s">
-        <v>48</v>
+      <c r="B7" s="71" t="s">
+        <v>123</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
       <c r="G7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1593,7 +1594,7 @@
     </row>
     <row r="9" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="52"/>
       <c r="D9" s="49"/>
@@ -1653,7 +1654,7 @@
       <c r="C10" s="55"/>
       <c r="D10" s="57"/>
       <c r="E10" s="50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
@@ -1707,7 +1708,7 @@
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B12" s="54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="2:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1724,31 +1725,31 @@
         <v>45</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="62" t="s">
+      <c r="B15" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="36">
         <v>1</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",FALSE,G15,E15,F15)</f>
@@ -1756,8 +1757,8 @@
       </c>
     </row>
     <row r="16" spans="2:51" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
-      <c r="C16" s="63"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" ref="H16:H61" si="0">_xlfn.TEXTJOIN(",",FALSE,G16,E16,F16)</f>
@@ -1774,17 +1775,17 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
-      <c r="C17" s="63"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="36">
         <v>0.5</v>
       </c>
       <c r="G17" s="47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1792,17 +1793,17 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="37">
         <v>0.5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1810,19 +1811,19 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
-      <c r="C19" s="62" t="s">
+      <c r="B19" s="68"/>
+      <c r="C19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="36">
         <v>1</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1830,17 +1831,17 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="58"/>
-      <c r="C20" s="63"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="62"/>
       <c r="D20" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="38">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1848,10 +1849,10 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1862,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1870,17 +1871,17 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="37">
         <v>0.5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1888,17 +1889,17 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="36">
         <v>0.5</v>
       </c>
       <c r="G23" s="47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1906,8 +1907,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1924,21 +1925,21 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="41">
         <v>1</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1946,8 +1947,8 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="58"/>
-      <c r="C26" s="63"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="6" t="s">
         <v>39</v>
       </c>
@@ -1956,7 +1957,7 @@
         <v>0.5</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1964,8 +1965,8 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="C27" s="63"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="10" t="s">
         <v>38</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1982,17 +1983,17 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="58"/>
-      <c r="C28" s="64"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="37">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2000,8 +2001,8 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="58"/>
-      <c r="C29" s="62" t="s">
+      <c r="B29" s="68"/>
+      <c r="C29" s="64" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
@@ -2012,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2020,8 +2021,8 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="58"/>
-      <c r="C30" s="63"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="6" t="s">
         <v>33</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2038,8 +2039,8 @@
       </c>
     </row>
     <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="58"/>
-      <c r="C31" s="64"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="10" t="s">
         <v>41</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2056,19 +2057,19 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="58"/>
-      <c r="C32" s="62" t="s">
+      <c r="B32" s="68"/>
+      <c r="C32" s="64" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="37">
         <v>0.25</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2076,17 +2077,17 @@
       </c>
     </row>
     <row r="33" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="58"/>
-      <c r="C33" s="63"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="36">
         <v>0.25</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2094,17 +2095,17 @@
       </c>
     </row>
     <row r="34" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="58"/>
-      <c r="C34" s="63"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34" s="37">
         <v>0.25</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2112,17 +2113,17 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="58"/>
-      <c r="C35" s="63"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="36">
         <v>0.25</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2130,8 +2131,8 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="58"/>
-      <c r="C36" s="63"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2148,8 +2149,8 @@
       </c>
     </row>
     <row r="37" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="58"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="10" t="s">
         <v>40</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2166,8 +2167,8 @@
       </c>
     </row>
     <row r="38" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="58"/>
-      <c r="C38" s="63"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="6" t="s">
         <v>36</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2184,17 +2185,17 @@
       </c>
     </row>
     <row r="39" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="58"/>
-      <c r="C39" s="63"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="62"/>
       <c r="D39" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="36">
         <v>1</v>
       </c>
       <c r="G39" s="47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2202,17 +2203,17 @@
       </c>
     </row>
     <row r="40" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="58"/>
-      <c r="C40" s="63"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="37">
         <v>0.5</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2220,17 +2221,17 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="58"/>
-      <c r="C41" s="63"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="42">
         <v>0.5</v>
       </c>
       <c r="G41" s="47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2241,7 +2242,7 @@
       <c r="B42" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -2252,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2262,7 @@
     </row>
     <row r="43" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="60"/>
-      <c r="C43" s="63"/>
+      <c r="C43" s="62"/>
       <c r="D43" s="10" t="s">
         <v>15</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2279,7 +2280,7 @@
     </row>
     <row r="44" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="60"/>
-      <c r="C44" s="64"/>
+      <c r="C44" s="63"/>
       <c r="D44" s="6" t="s">
         <v>16</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2297,7 +2298,7 @@
     </row>
     <row r="45" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="60"/>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="64" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -2308,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2317,16 +2318,16 @@
     </row>
     <row r="46" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="60"/>
-      <c r="C46" s="63"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="37">
         <v>0.5</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2335,16 +2336,16 @@
     </row>
     <row r="47" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="60"/>
-      <c r="C47" s="63"/>
+      <c r="C47" s="62"/>
       <c r="D47" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="36">
         <v>0.5</v>
       </c>
       <c r="G47" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2353,7 +2354,7 @@
     </row>
     <row r="48" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="60"/>
-      <c r="C48" s="64"/>
+      <c r="C48" s="63"/>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2371,7 +2372,7 @@
     </row>
     <row r="49" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="60"/>
-      <c r="C49" s="62" t="s">
+      <c r="C49" s="64" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="10" t="s">
@@ -2382,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2391,7 +2392,7 @@
     </row>
     <row r="50" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="60"/>
-      <c r="C50" s="63"/>
+      <c r="C50" s="62"/>
       <c r="D50" s="6" t="s">
         <v>22</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2409,16 +2410,16 @@
     </row>
     <row r="51" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="61"/>
-      <c r="C51" s="68"/>
+      <c r="C51" s="66"/>
       <c r="D51" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E51" s="33"/>
       <c r="F51" s="44">
         <v>1</v>
       </c>
       <c r="G51" s="47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2429,7 +2430,7 @@
       <c r="B52" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="63" t="s">
+      <c r="C52" s="62" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="8" t="s">
@@ -2440,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2449,7 +2450,7 @@
     </row>
     <row r="53" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="60"/>
-      <c r="C53" s="63"/>
+      <c r="C53" s="62"/>
       <c r="D53" s="10" t="s">
         <v>25</v>
       </c>
@@ -2458,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2467,7 +2468,7 @@
     </row>
     <row r="54" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="60"/>
-      <c r="C54" s="63"/>
+      <c r="C54" s="62"/>
       <c r="D54" s="6" t="s">
         <v>34</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>0.5</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2485,7 +2486,7 @@
     </row>
     <row r="55" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="60"/>
-      <c r="C55" s="64"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="10" t="s">
         <v>26</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>0.5</v>
       </c>
       <c r="G55" s="47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2503,7 +2504,7 @@
     </row>
     <row r="56" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="60"/>
-      <c r="C56" s="62" t="s">
+      <c r="C56" s="64" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -2514,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2523,7 +2524,7 @@
     </row>
     <row r="57" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="60"/>
-      <c r="C57" s="63"/>
+      <c r="C57" s="62"/>
       <c r="D57" s="10" t="s">
         <v>44</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2541,16 +2542,16 @@
     </row>
     <row r="58" spans="2:8" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B58" s="60"/>
-      <c r="C58" s="63"/>
+      <c r="C58" s="62"/>
       <c r="D58" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="38">
         <v>1</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2572,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2583,14 +2584,14 @@
       <c r="B60" s="60"/>
       <c r="C60" s="60"/>
       <c r="D60" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E60" s="26"/>
       <c r="F60" s="37">
         <v>1</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2608,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="47" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2754,6 +2755,9 @@
     <row r="198" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B20"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="C25:C28"/>
@@ -2770,9 +2774,6 @@
     <mergeCell ref="B25:B41"/>
     <mergeCell ref="B42:B51"/>
     <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B20"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>